<commit_message>
Database Methods vs DML Statements
</commit_message>
<xml_diff>
--- a/me/7.SObject-and-DML.xlsx
+++ b/me/7.SObject-and-DML.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97B4CDE-C7EA-4A95-B183-EFC6E87223F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B508A0E4-62F7-432E-9F11-20CE3E7B474D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Insert Operation" sheetId="1" r:id="rId1"/>
     <sheet name="DML Logs Discussion" sheetId="2" r:id="rId2"/>
+    <sheet name="DatabaseMethodsVsDML Statements" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -460,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -473,8 +474,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2460,6 +2459,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>27257</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40AE36FC-D523-5A9F-7842-C6A5DFDC7F15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="685800"/>
+          <a:ext cx="11096625" cy="5056457"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5325,7 +5373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8367AB-9157-40B0-A1ED-CB33FE7AD93F}">
   <dimension ref="A4:T255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
+    <sheetView topLeftCell="A256" workbookViewId="0">
       <selection activeCell="G136" sqref="G136"/>
     </sheetView>
   </sheetViews>
@@ -5386,37 +5434,29 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
-      <c r="C11" s="12" t="s">
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
       <c r="F11" s="7"/>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12" t="s">
+      <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="12"/>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12" t="s">
+      <c r="E13" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12" t="s">
+      <c r="E14" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="6"/>
@@ -5482,451 +5522,206 @@
       <c r="B22" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
       <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
       <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
       <c r="J28" s="6"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
       <c r="J29" s="6"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
       <c r="J30" s="6"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
       <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
       <c r="J32" s="6"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
       <c r="J33" s="6"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
       <c r="J34" s="6"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
       <c r="J36" s="6"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
       <c r="J38" s="6"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
       <c r="J39" s="6"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
       <c r="J40" s="6"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
       <c r="J43" s="6"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
       <c r="J44" s="6"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
       <c r="J45" s="6"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
       <c r="J46" s="6"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
       <c r="J47" s="6"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
       <c r="J48" s="6"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
       <c r="J49" s="6"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
       <c r="J50" s="6"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
       <c r="J51" s="6"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
       <c r="J52" s="6"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
       <c r="J53" s="6"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
       <c r="J54" s="6"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
       <c r="J55" s="6"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
       <c r="J56" s="6"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
@@ -5976,16 +5771,6 @@
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="4"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
-      <c r="K61" s="13"/>
-      <c r="L61" s="13"/>
-      <c r="M61" s="13"/>
-      <c r="N61" s="13"/>
-      <c r="O61" s="13"/>
-      <c r="P61" s="13"/>
-      <c r="Q61" s="13"/>
-      <c r="R61" s="13"/>
       <c r="S61" s="6"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
@@ -5993,22 +5778,7 @@
       <c r="B62" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
       <c r="H62" s="6"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
-      <c r="N62" s="13"/>
-      <c r="O62" s="13"/>
-      <c r="P62" s="13"/>
-      <c r="Q62" s="13"/>
-      <c r="R62" s="13"/>
       <c r="S62" s="6"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
@@ -6016,22 +5786,7 @@
       <c r="B63" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
       <c r="H63" s="6"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="13"/>
-      <c r="N63" s="13"/>
-      <c r="O63" s="13"/>
-      <c r="P63" s="13"/>
-      <c r="Q63" s="13"/>
-      <c r="R63" s="13"/>
       <c r="S63" s="6"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
@@ -6039,22 +5794,7 @@
       <c r="B64" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
       <c r="H64" s="6"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13"/>
-      <c r="K64" s="13"/>
-      <c r="L64" s="13"/>
-      <c r="M64" s="13"/>
-      <c r="N64" s="13"/>
-      <c r="O64" s="13"/>
-      <c r="P64" s="13"/>
-      <c r="Q64" s="13"/>
-      <c r="R64" s="13"/>
       <c r="S64" s="6"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
@@ -6062,22 +5802,7 @@
       <c r="B65" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
       <c r="H65" s="6"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="13"/>
-      <c r="K65" s="13"/>
-      <c r="L65" s="13"/>
-      <c r="M65" s="13"/>
-      <c r="N65" s="13"/>
-      <c r="O65" s="13"/>
-      <c r="P65" s="13"/>
-      <c r="Q65" s="13"/>
-      <c r="R65" s="13"/>
       <c r="S65" s="6"/>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
@@ -6085,22 +5810,7 @@
       <c r="B66" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
       <c r="H66" s="6"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="13"/>
-      <c r="K66" s="13"/>
-      <c r="L66" s="13"/>
-      <c r="M66" s="13"/>
-      <c r="N66" s="13"/>
-      <c r="O66" s="13"/>
-      <c r="P66" s="13"/>
-      <c r="Q66" s="13"/>
-      <c r="R66" s="13"/>
       <c r="S66" s="6"/>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
@@ -6108,22 +5818,7 @@
       <c r="B67" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
       <c r="H67" s="6"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="13"/>
-      <c r="M67" s="13"/>
-      <c r="N67" s="13"/>
-      <c r="O67" s="13"/>
-      <c r="P67" s="13"/>
-      <c r="Q67" s="13"/>
-      <c r="R67" s="13"/>
       <c r="S67" s="6"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
@@ -6131,22 +5826,7 @@
       <c r="B68" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="13"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
       <c r="H68" s="6"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="13"/>
-      <c r="K68" s="13"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="13"/>
-      <c r="N68" s="13"/>
-      <c r="O68" s="13"/>
-      <c r="P68" s="13"/>
-      <c r="Q68" s="13"/>
-      <c r="R68" s="13"/>
       <c r="S68" s="6"/>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
@@ -6154,22 +5834,7 @@
       <c r="B69" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
       <c r="H69" s="6"/>
-      <c r="I69" s="13"/>
-      <c r="J69" s="13"/>
-      <c r="K69" s="13"/>
-      <c r="L69" s="13"/>
-      <c r="M69" s="13"/>
-      <c r="N69" s="13"/>
-      <c r="O69" s="13"/>
-      <c r="P69" s="13"/>
-      <c r="Q69" s="13"/>
-      <c r="R69" s="13"/>
       <c r="S69" s="6"/>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
@@ -6177,22 +5842,7 @@
       <c r="B70" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
       <c r="H70" s="6"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-      <c r="L70" s="13"/>
-      <c r="M70" s="13"/>
-      <c r="N70" s="13"/>
-      <c r="O70" s="13"/>
-      <c r="P70" s="13"/>
-      <c r="Q70" s="13"/>
-      <c r="R70" s="13"/>
       <c r="S70" s="6"/>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
@@ -6200,22 +5850,7 @@
       <c r="B71" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="13"/>
       <c r="H71" s="6"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
-      <c r="L71" s="13"/>
-      <c r="M71" s="13"/>
-      <c r="N71" s="13"/>
-      <c r="O71" s="13"/>
-      <c r="P71" s="13"/>
-      <c r="Q71" s="13"/>
-      <c r="R71" s="13"/>
       <c r="S71" s="6"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
@@ -6223,22 +5858,7 @@
       <c r="B72" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
       <c r="H72" s="6"/>
-      <c r="I72" s="13"/>
-      <c r="J72" s="13"/>
-      <c r="K72" s="13"/>
-      <c r="L72" s="13"/>
-      <c r="M72" s="13"/>
-      <c r="N72" s="13"/>
-      <c r="O72" s="13"/>
-      <c r="P72" s="13"/>
-      <c r="Q72" s="13"/>
-      <c r="R72" s="13"/>
       <c r="S72" s="6"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
@@ -6246,22 +5866,7 @@
       <c r="B73" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="13"/>
       <c r="H73" s="6"/>
-      <c r="I73" s="13"/>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
-      <c r="L73" s="13"/>
-      <c r="M73" s="13"/>
-      <c r="N73" s="13"/>
-      <c r="O73" s="13"/>
-      <c r="P73" s="13"/>
-      <c r="Q73" s="13"/>
-      <c r="R73" s="13"/>
       <c r="S73" s="6"/>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
@@ -6269,22 +5874,7 @@
       <c r="B74" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
       <c r="H74" s="6"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
-      <c r="L74" s="13"/>
-      <c r="M74" s="13"/>
-      <c r="N74" s="13"/>
-      <c r="O74" s="13"/>
-      <c r="P74" s="13"/>
-      <c r="Q74" s="13"/>
-      <c r="R74" s="13"/>
       <c r="S74" s="6"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
@@ -6298,1257 +5888,245 @@
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
       <c r="H75" s="10"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
-      <c r="L75" s="13"/>
-      <c r="M75" s="13"/>
-      <c r="N75" s="13"/>
-      <c r="O75" s="13"/>
-      <c r="P75" s="13"/>
-      <c r="Q75" s="13"/>
-      <c r="R75" s="13"/>
       <c r="S75" s="6"/>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="13"/>
-      <c r="K76" s="13"/>
-      <c r="L76" s="13"/>
-      <c r="M76" s="13"/>
-      <c r="N76" s="13"/>
-      <c r="O76" s="13"/>
-      <c r="P76" s="13"/>
-      <c r="Q76" s="13"/>
-      <c r="R76" s="13"/>
       <c r="S76" s="6"/>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="13"/>
-      <c r="K77" s="13"/>
-      <c r="L77" s="13"/>
-      <c r="M77" s="13"/>
-      <c r="N77" s="13"/>
-      <c r="O77" s="13"/>
-      <c r="P77" s="13"/>
-      <c r="Q77" s="13"/>
-      <c r="R77" s="13"/>
       <c r="S77" s="6"/>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="13"/>
-      <c r="E78" s="13"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="13"/>
-      <c r="H78" s="13"/>
-      <c r="I78" s="13"/>
-      <c r="J78" s="13"/>
-      <c r="K78" s="13"/>
-      <c r="L78" s="13"/>
-      <c r="M78" s="13"/>
-      <c r="N78" s="13"/>
-      <c r="O78" s="13"/>
-      <c r="P78" s="13"/>
-      <c r="Q78" s="13"/>
-      <c r="R78" s="13"/>
       <c r="S78" s="6"/>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="13"/>
-      <c r="J79" s="13"/>
-      <c r="K79" s="13"/>
-      <c r="L79" s="13"/>
-      <c r="M79" s="13"/>
-      <c r="N79" s="13"/>
-      <c r="O79" s="13"/>
-      <c r="P79" s="13"/>
-      <c r="Q79" s="13"/>
-      <c r="R79" s="13"/>
       <c r="S79" s="6"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
-      <c r="J80" s="13"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="13"/>
-      <c r="M80" s="13"/>
-      <c r="N80" s="13"/>
-      <c r="O80" s="13"/>
-      <c r="P80" s="13"/>
-      <c r="Q80" s="13"/>
-      <c r="R80" s="13"/>
       <c r="S80" s="6"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="13"/>
-      <c r="K81" s="13"/>
-      <c r="L81" s="13"/>
-      <c r="M81" s="13"/>
-      <c r="N81" s="13"/>
-      <c r="O81" s="13"/>
-      <c r="P81" s="13"/>
-      <c r="Q81" s="13"/>
-      <c r="R81" s="13"/>
       <c r="S81" s="6"/>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="13"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="13"/>
-      <c r="K82" s="13"/>
-      <c r="L82" s="13"/>
-      <c r="M82" s="13"/>
-      <c r="N82" s="13"/>
-      <c r="O82" s="13"/>
-      <c r="P82" s="13"/>
-      <c r="Q82" s="13"/>
-      <c r="R82" s="13"/>
       <c r="S82" s="6"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13"/>
-      <c r="K83" s="13"/>
-      <c r="L83" s="13"/>
-      <c r="M83" s="13"/>
-      <c r="N83" s="13"/>
-      <c r="O83" s="13"/>
-      <c r="P83" s="13"/>
-      <c r="Q83" s="13"/>
-      <c r="R83" s="13"/>
       <c r="S83" s="6"/>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="13"/>
-      <c r="K84" s="13"/>
-      <c r="L84" s="13"/>
-      <c r="M84" s="13"/>
-      <c r="N84" s="13"/>
-      <c r="O84" s="13"/>
-      <c r="P84" s="13"/>
-      <c r="Q84" s="13"/>
-      <c r="R84" s="13"/>
       <c r="S84" s="6"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
-      <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="13"/>
-      <c r="E85" s="13"/>
-      <c r="F85" s="13"/>
-      <c r="G85" s="13"/>
-      <c r="H85" s="13"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="13"/>
-      <c r="K85" s="13"/>
-      <c r="L85" s="13"/>
-      <c r="M85" s="13"/>
-      <c r="N85" s="13"/>
-      <c r="O85" s="13"/>
-      <c r="P85" s="13"/>
-      <c r="Q85" s="13"/>
-      <c r="R85" s="13"/>
       <c r="S85" s="6"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
-      <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13"/>
-      <c r="K86" s="13"/>
-      <c r="L86" s="13"/>
-      <c r="M86" s="13"/>
-      <c r="N86" s="13"/>
-      <c r="O86" s="13"/>
-      <c r="P86" s="13"/>
-      <c r="Q86" s="13"/>
-      <c r="R86" s="13"/>
       <c r="S86" s="6"/>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="13"/>
-      <c r="K87" s="13"/>
-      <c r="L87" s="13"/>
-      <c r="M87" s="13"/>
-      <c r="N87" s="13"/>
-      <c r="O87" s="13"/>
-      <c r="P87" s="13"/>
-      <c r="Q87" s="13"/>
-      <c r="R87" s="13"/>
       <c r="S87" s="6"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="13"/>
-      <c r="J88" s="13"/>
-      <c r="K88" s="13"/>
-      <c r="L88" s="13"/>
-      <c r="M88" s="13"/>
-      <c r="N88" s="13"/>
-      <c r="O88" s="13"/>
-      <c r="P88" s="13"/>
-      <c r="Q88" s="13"/>
-      <c r="R88" s="13"/>
       <c r="S88" s="6"/>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
-      <c r="B89" s="13"/>
-      <c r="C89" s="13"/>
-      <c r="D89" s="13"/>
-      <c r="E89" s="13"/>
-      <c r="F89" s="13"/>
-      <c r="G89" s="13"/>
-      <c r="H89" s="13"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="13"/>
-      <c r="K89" s="13"/>
-      <c r="L89" s="13"/>
-      <c r="M89" s="13"/>
-      <c r="N89" s="13"/>
-      <c r="O89" s="13"/>
-      <c r="P89" s="13"/>
-      <c r="Q89" s="13"/>
-      <c r="R89" s="13"/>
       <c r="S89" s="6"/>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
-      <c r="E90" s="13"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="13"/>
-      <c r="K90" s="13"/>
-      <c r="L90" s="13"/>
-      <c r="M90" s="13"/>
-      <c r="N90" s="13"/>
-      <c r="O90" s="13"/>
-      <c r="P90" s="13"/>
-      <c r="Q90" s="13"/>
-      <c r="R90" s="13"/>
       <c r="S90" s="6"/>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
-      <c r="B91" s="13"/>
-      <c r="C91" s="13"/>
-      <c r="D91" s="13"/>
-      <c r="E91" s="13"/>
-      <c r="F91" s="13"/>
-      <c r="G91" s="13"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13"/>
-      <c r="K91" s="13"/>
-      <c r="L91" s="13"/>
-      <c r="M91" s="13"/>
-      <c r="N91" s="13"/>
-      <c r="O91" s="13"/>
-      <c r="P91" s="13"/>
-      <c r="Q91" s="13"/>
-      <c r="R91" s="13"/>
       <c r="S91" s="6"/>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
-      <c r="B92" s="13"/>
-      <c r="C92" s="13"/>
-      <c r="D92" s="13"/>
-      <c r="E92" s="13"/>
-      <c r="F92" s="13"/>
-      <c r="G92" s="13"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13"/>
-      <c r="K92" s="13"/>
-      <c r="L92" s="13"/>
-      <c r="M92" s="13"/>
-      <c r="N92" s="13"/>
-      <c r="O92" s="13"/>
-      <c r="P92" s="13"/>
-      <c r="Q92" s="13"/>
-      <c r="R92" s="13"/>
       <c r="S92" s="6"/>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
-      <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
-      <c r="D93" s="13"/>
-      <c r="E93" s="13"/>
-      <c r="F93" s="13"/>
-      <c r="G93" s="13"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="13"/>
-      <c r="K93" s="13"/>
-      <c r="L93" s="13"/>
-      <c r="M93" s="13"/>
-      <c r="N93" s="13"/>
-      <c r="O93" s="13"/>
-      <c r="P93" s="13"/>
-      <c r="Q93" s="13"/>
-      <c r="R93" s="13"/>
       <c r="S93" s="6"/>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
-      <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
-      <c r="D94" s="13"/>
-      <c r="E94" s="13"/>
-      <c r="F94" s="13"/>
-      <c r="G94" s="13"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="13"/>
-      <c r="J94" s="13"/>
-      <c r="K94" s="13"/>
-      <c r="L94" s="13"/>
-      <c r="M94" s="13"/>
-      <c r="N94" s="13"/>
-      <c r="O94" s="13"/>
-      <c r="P94" s="13"/>
-      <c r="Q94" s="13"/>
-      <c r="R94" s="13"/>
       <c r="S94" s="6"/>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
-      <c r="B95" s="13"/>
-      <c r="C95" s="13"/>
-      <c r="D95" s="13"/>
-      <c r="E95" s="13"/>
-      <c r="F95" s="13"/>
-      <c r="G95" s="13"/>
-      <c r="H95" s="13"/>
-      <c r="I95" s="13"/>
-      <c r="J95" s="13"/>
-      <c r="K95" s="13"/>
-      <c r="L95" s="13"/>
-      <c r="M95" s="13"/>
-      <c r="N95" s="13"/>
-      <c r="O95" s="13"/>
-      <c r="P95" s="13"/>
-      <c r="Q95" s="13"/>
-      <c r="R95" s="13"/>
       <c r="S95" s="6"/>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
-      <c r="B96" s="13"/>
-      <c r="C96" s="13"/>
-      <c r="D96" s="13"/>
-      <c r="E96" s="13"/>
-      <c r="F96" s="13"/>
-      <c r="G96" s="13"/>
-      <c r="H96" s="13"/>
-      <c r="I96" s="13"/>
-      <c r="J96" s="13"/>
-      <c r="K96" s="13"/>
-      <c r="L96" s="13"/>
-      <c r="M96" s="13"/>
-      <c r="N96" s="13"/>
-      <c r="O96" s="13"/>
-      <c r="P96" s="13"/>
-      <c r="Q96" s="13"/>
-      <c r="R96" s="13"/>
       <c r="S96" s="6"/>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
-      <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
-      <c r="D97" s="13"/>
-      <c r="E97" s="13"/>
-      <c r="F97" s="13"/>
-      <c r="G97" s="13"/>
-      <c r="H97" s="13"/>
-      <c r="I97" s="13"/>
-      <c r="J97" s="13"/>
-      <c r="K97" s="13"/>
-      <c r="L97" s="13"/>
-      <c r="M97" s="13"/>
-      <c r="N97" s="13"/>
-      <c r="O97" s="13"/>
-      <c r="P97" s="13"/>
-      <c r="Q97" s="13"/>
-      <c r="R97" s="13"/>
       <c r="S97" s="6"/>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="13"/>
-      <c r="J98" s="13"/>
-      <c r="K98" s="13"/>
-      <c r="L98" s="13"/>
-      <c r="M98" s="13"/>
-      <c r="N98" s="13"/>
-      <c r="O98" s="13"/>
-      <c r="P98" s="13"/>
-      <c r="Q98" s="13"/>
-      <c r="R98" s="13"/>
       <c r="S98" s="6"/>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
-      <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
-      <c r="D99" s="13"/>
-      <c r="E99" s="13"/>
-      <c r="F99" s="13"/>
-      <c r="G99" s="13"/>
-      <c r="H99" s="13"/>
-      <c r="I99" s="13"/>
-      <c r="J99" s="13"/>
-      <c r="K99" s="13"/>
-      <c r="L99" s="13"/>
-      <c r="M99" s="13"/>
-      <c r="N99" s="13"/>
-      <c r="O99" s="13"/>
-      <c r="P99" s="13"/>
-      <c r="Q99" s="13"/>
-      <c r="R99" s="13"/>
       <c r="S99" s="6"/>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
-      <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
-      <c r="D100" s="13"/>
-      <c r="E100" s="13"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
-      <c r="J100" s="13"/>
-      <c r="K100" s="13"/>
-      <c r="L100" s="13"/>
-      <c r="M100" s="13"/>
-      <c r="N100" s="13"/>
-      <c r="O100" s="13"/>
-      <c r="P100" s="13"/>
-      <c r="Q100" s="13"/>
-      <c r="R100" s="13"/>
       <c r="S100" s="6"/>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
-      <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
-      <c r="D101" s="13"/>
-      <c r="E101" s="13"/>
-      <c r="F101" s="13"/>
-      <c r="G101" s="13"/>
-      <c r="H101" s="13"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="13"/>
-      <c r="K101" s="13"/>
-      <c r="L101" s="13"/>
-      <c r="M101" s="13"/>
-      <c r="N101" s="13"/>
-      <c r="O101" s="13"/>
-      <c r="P101" s="13"/>
-      <c r="Q101" s="13"/>
-      <c r="R101" s="13"/>
       <c r="S101" s="6"/>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
-      <c r="B102" s="13"/>
-      <c r="C102" s="13"/>
-      <c r="D102" s="13"/>
-      <c r="E102" s="13"/>
-      <c r="F102" s="13"/>
-      <c r="G102" s="13"/>
-      <c r="H102" s="13"/>
-      <c r="I102" s="13"/>
-      <c r="J102" s="13"/>
-      <c r="K102" s="13"/>
-      <c r="L102" s="13"/>
-      <c r="M102" s="13"/>
-      <c r="N102" s="13"/>
-      <c r="O102" s="13"/>
-      <c r="P102" s="13"/>
-      <c r="Q102" s="13"/>
-      <c r="R102" s="13"/>
       <c r="S102" s="6"/>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
-      <c r="B103" s="13"/>
-      <c r="C103" s="13"/>
-      <c r="D103" s="13"/>
-      <c r="E103" s="13"/>
-      <c r="F103" s="13"/>
-      <c r="G103" s="13"/>
-      <c r="H103" s="13"/>
-      <c r="I103" s="13"/>
-      <c r="J103" s="13"/>
-      <c r="K103" s="13"/>
-      <c r="L103" s="13"/>
-      <c r="M103" s="13"/>
-      <c r="N103" s="13"/>
-      <c r="O103" s="13"/>
-      <c r="P103" s="13"/>
-      <c r="Q103" s="13"/>
-      <c r="R103" s="13"/>
       <c r="S103" s="6"/>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
-      <c r="B104" s="13"/>
-      <c r="C104" s="13"/>
-      <c r="D104" s="13"/>
-      <c r="E104" s="13"/>
-      <c r="F104" s="13"/>
-      <c r="G104" s="13"/>
-      <c r="H104" s="13"/>
-      <c r="I104" s="13"/>
-      <c r="J104" s="13"/>
-      <c r="K104" s="13"/>
-      <c r="L104" s="13"/>
-      <c r="M104" s="13"/>
-      <c r="N104" s="13"/>
-      <c r="O104" s="13"/>
-      <c r="P104" s="13"/>
-      <c r="Q104" s="13"/>
-      <c r="R104" s="13"/>
       <c r="S104" s="6"/>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
-      <c r="B105" s="13"/>
-      <c r="C105" s="13"/>
-      <c r="D105" s="13"/>
-      <c r="E105" s="13"/>
-      <c r="F105" s="13"/>
-      <c r="G105" s="13"/>
-      <c r="H105" s="13"/>
-      <c r="I105" s="13"/>
-      <c r="J105" s="13"/>
-      <c r="K105" s="13"/>
-      <c r="L105" s="13"/>
-      <c r="M105" s="13"/>
-      <c r="N105" s="13"/>
-      <c r="O105" s="13"/>
-      <c r="P105" s="13"/>
-      <c r="Q105" s="13"/>
-      <c r="R105" s="13"/>
       <c r="S105" s="6"/>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
-      <c r="B106" s="13" t="s">
+      <c r="B106" t="s">
         <v>98</v>
       </c>
-      <c r="C106" s="13"/>
-      <c r="D106" s="13"/>
-      <c r="E106" s="13"/>
-      <c r="F106" s="13"/>
-      <c r="G106" s="13"/>
-      <c r="H106" s="13"/>
-      <c r="I106" s="13"/>
-      <c r="J106" s="13"/>
-      <c r="K106" s="13"/>
-      <c r="L106" s="13"/>
-      <c r="M106" s="13"/>
-      <c r="N106" s="13"/>
-      <c r="O106" s="13"/>
-      <c r="P106" s="13"/>
-      <c r="Q106" s="13"/>
-      <c r="R106" s="13"/>
       <c r="S106" s="6"/>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
-      <c r="B107" s="13"/>
-      <c r="C107" s="13"/>
-      <c r="D107" s="13"/>
-      <c r="E107" s="13"/>
-      <c r="F107" s="13"/>
-      <c r="G107" s="13"/>
-      <c r="H107" s="13"/>
-      <c r="I107" s="13"/>
-      <c r="J107" s="13"/>
-      <c r="K107" s="13"/>
-      <c r="L107" s="13"/>
-      <c r="M107" s="13"/>
-      <c r="N107" s="13"/>
-      <c r="O107" s="13"/>
-      <c r="P107" s="13"/>
-      <c r="Q107" s="13"/>
-      <c r="R107" s="13"/>
       <c r="S107" s="6"/>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
-      <c r="B108" s="13"/>
-      <c r="C108" s="13"/>
-      <c r="D108" s="13"/>
-      <c r="E108" s="13"/>
-      <c r="F108" s="13"/>
-      <c r="G108" s="13"/>
-      <c r="H108" s="13"/>
-      <c r="I108" s="13"/>
-      <c r="J108" s="13"/>
-      <c r="K108" s="13"/>
-      <c r="L108" s="13"/>
-      <c r="M108" s="13"/>
-      <c r="N108" s="13"/>
-      <c r="O108" s="13"/>
-      <c r="P108" s="13"/>
-      <c r="Q108" s="13"/>
-      <c r="R108" s="13"/>
       <c r="S108" s="6"/>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
-      <c r="B109" s="13"/>
-      <c r="C109" s="13"/>
-      <c r="D109" s="13"/>
-      <c r="E109" s="13"/>
-      <c r="F109" s="13"/>
-      <c r="G109" s="13"/>
-      <c r="H109" s="13"/>
-      <c r="I109" s="13"/>
-      <c r="J109" s="13"/>
-      <c r="K109" s="13"/>
-      <c r="L109" s="13"/>
-      <c r="M109" s="13"/>
-      <c r="N109" s="13"/>
-      <c r="O109" s="13"/>
-      <c r="P109" s="13"/>
-      <c r="Q109" s="13"/>
-      <c r="R109" s="13"/>
       <c r="S109" s="6"/>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
-      <c r="B110" s="13"/>
-      <c r="C110" s="13"/>
-      <c r="D110" s="13"/>
-      <c r="E110" s="13"/>
-      <c r="F110" s="13"/>
-      <c r="G110" s="13"/>
-      <c r="H110" s="13"/>
-      <c r="I110" s="13"/>
-      <c r="J110" s="13"/>
-      <c r="K110" s="13"/>
-      <c r="L110" s="13"/>
-      <c r="M110" s="13"/>
-      <c r="N110" s="13"/>
-      <c r="O110" s="13"/>
-      <c r="P110" s="13"/>
-      <c r="Q110" s="13"/>
-      <c r="R110" s="13"/>
       <c r="S110" s="6"/>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
-      <c r="B111" s="13"/>
-      <c r="C111" s="13"/>
-      <c r="D111" s="13"/>
-      <c r="E111" s="13"/>
-      <c r="F111" s="13"/>
-      <c r="G111" s="13"/>
-      <c r="H111" s="13"/>
-      <c r="I111" s="13"/>
-      <c r="J111" s="13"/>
-      <c r="K111" s="13"/>
-      <c r="L111" s="13"/>
-      <c r="M111" s="13"/>
-      <c r="N111" s="13"/>
-      <c r="O111" s="13"/>
-      <c r="P111" s="13"/>
-      <c r="Q111" s="13"/>
-      <c r="R111" s="13"/>
       <c r="S111" s="6"/>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
-      <c r="B112" s="13"/>
-      <c r="C112" s="13"/>
-      <c r="D112" s="13"/>
-      <c r="E112" s="13"/>
-      <c r="F112" s="13"/>
-      <c r="G112" s="13"/>
-      <c r="H112" s="13"/>
-      <c r="I112" s="13"/>
-      <c r="J112" s="13"/>
-      <c r="K112" s="13"/>
-      <c r="L112" s="13"/>
-      <c r="M112" s="13"/>
-      <c r="N112" s="13"/>
-      <c r="O112" s="13"/>
-      <c r="P112" s="13"/>
-      <c r="Q112" s="13"/>
-      <c r="R112" s="13"/>
       <c r="S112" s="6"/>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
-      <c r="B113" s="13"/>
-      <c r="C113" s="13"/>
-      <c r="D113" s="13"/>
-      <c r="E113" s="13"/>
-      <c r="F113" s="13"/>
-      <c r="G113" s="13"/>
-      <c r="H113" s="13"/>
-      <c r="I113" s="13"/>
-      <c r="J113" s="13"/>
-      <c r="K113" s="13"/>
-      <c r="L113" s="13"/>
-      <c r="M113" s="13"/>
-      <c r="N113" s="13"/>
-      <c r="O113" s="13"/>
-      <c r="P113" s="13"/>
-      <c r="Q113" s="13"/>
-      <c r="R113" s="13"/>
       <c r="S113" s="6"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
-      <c r="B114" s="13"/>
-      <c r="C114" s="13"/>
-      <c r="D114" s="13"/>
-      <c r="E114" s="13"/>
-      <c r="F114" s="13"/>
-      <c r="G114" s="13"/>
-      <c r="H114" s="13"/>
-      <c r="I114" s="13"/>
-      <c r="J114" s="13"/>
-      <c r="K114" s="13"/>
-      <c r="L114" s="13"/>
-      <c r="M114" s="13"/>
-      <c r="N114" s="13"/>
-      <c r="O114" s="13"/>
-      <c r="P114" s="13"/>
-      <c r="Q114" s="13"/>
-      <c r="R114" s="13"/>
       <c r="S114" s="6"/>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
-      <c r="B115" s="13"/>
-      <c r="C115" s="13"/>
-      <c r="D115" s="13"/>
-      <c r="E115" s="13"/>
-      <c r="F115" s="13"/>
-      <c r="G115" s="13"/>
-      <c r="H115" s="13"/>
-      <c r="I115" s="13"/>
-      <c r="J115" s="13"/>
-      <c r="K115" s="13"/>
-      <c r="L115" s="13"/>
-      <c r="M115" s="13"/>
-      <c r="N115" s="13"/>
-      <c r="O115" s="13"/>
-      <c r="P115" s="13"/>
-      <c r="Q115" s="13"/>
-      <c r="R115" s="13"/>
       <c r="S115" s="6"/>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
-      <c r="B116" s="13"/>
-      <c r="C116" s="13"/>
-      <c r="D116" s="13"/>
-      <c r="E116" s="13"/>
-      <c r="F116" s="13"/>
-      <c r="G116" s="13"/>
-      <c r="H116" s="13"/>
-      <c r="I116" s="13"/>
-      <c r="J116" s="13"/>
-      <c r="K116" s="13"/>
-      <c r="L116" s="13"/>
-      <c r="M116" s="13"/>
-      <c r="N116" s="13"/>
-      <c r="O116" s="13"/>
-      <c r="P116" s="13"/>
-      <c r="Q116" s="13"/>
-      <c r="R116" s="13"/>
       <c r="S116" s="6"/>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
-      <c r="B117" s="13"/>
-      <c r="C117" s="13"/>
-      <c r="D117" s="13"/>
-      <c r="E117" s="13"/>
-      <c r="F117" s="13"/>
-      <c r="G117" s="13"/>
-      <c r="H117" s="13"/>
-      <c r="I117" s="13"/>
-      <c r="J117" s="13"/>
-      <c r="K117" s="13"/>
-      <c r="L117" s="13"/>
-      <c r="M117" s="13"/>
-      <c r="N117" s="13"/>
-      <c r="O117" s="13"/>
-      <c r="P117" s="13"/>
-      <c r="Q117" s="13"/>
-      <c r="R117" s="13"/>
       <c r="S117" s="6"/>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
-      <c r="B118" s="13"/>
-      <c r="C118" s="13"/>
-      <c r="D118" s="13"/>
-      <c r="E118" s="13"/>
-      <c r="F118" s="13"/>
-      <c r="G118" s="13"/>
-      <c r="H118" s="13"/>
-      <c r="I118" s="13"/>
-      <c r="J118" s="13"/>
-      <c r="K118" s="13"/>
-      <c r="L118" s="13"/>
-      <c r="M118" s="13"/>
-      <c r="N118" s="13"/>
-      <c r="O118" s="13"/>
-      <c r="P118" s="13"/>
-      <c r="Q118" s="13"/>
-      <c r="R118" s="13"/>
       <c r="S118" s="6"/>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
-      <c r="B119" s="13"/>
-      <c r="C119" s="13"/>
-      <c r="D119" s="13"/>
-      <c r="E119" s="13"/>
-      <c r="F119" s="13"/>
-      <c r="G119" s="13"/>
-      <c r="H119" s="13"/>
-      <c r="I119" s="13"/>
-      <c r="J119" s="13"/>
-      <c r="K119" s="13"/>
-      <c r="L119" s="13"/>
-      <c r="M119" s="13"/>
-      <c r="N119" s="13"/>
-      <c r="O119" s="13"/>
-      <c r="P119" s="13"/>
-      <c r="Q119" s="13"/>
-      <c r="R119" s="13"/>
       <c r="S119" s="6"/>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
-      <c r="B120" s="13"/>
-      <c r="C120" s="13"/>
-      <c r="D120" s="13"/>
-      <c r="E120" s="13"/>
-      <c r="F120" s="13"/>
-      <c r="G120" s="13"/>
-      <c r="H120" s="13"/>
-      <c r="I120" s="13"/>
-      <c r="J120" s="13"/>
-      <c r="K120" s="13"/>
-      <c r="L120" s="13"/>
-      <c r="M120" s="13"/>
-      <c r="N120" s="13"/>
-      <c r="O120" s="13"/>
-      <c r="P120" s="13"/>
-      <c r="Q120" s="13"/>
-      <c r="R120" s="13"/>
       <c r="S120" s="6"/>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
-      <c r="B121" s="13"/>
-      <c r="C121" s="13"/>
-      <c r="D121" s="13"/>
-      <c r="E121" s="13"/>
-      <c r="F121" s="13"/>
-      <c r="G121" s="13"/>
-      <c r="H121" s="13"/>
-      <c r="I121" s="13"/>
-      <c r="J121" s="13"/>
-      <c r="K121" s="13"/>
-      <c r="L121" s="13"/>
-      <c r="M121" s="13"/>
-      <c r="N121" s="13"/>
-      <c r="O121" s="13"/>
-      <c r="P121" s="13"/>
-      <c r="Q121" s="13"/>
-      <c r="R121" s="13"/>
       <c r="S121" s="6"/>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
-      <c r="B122" s="13"/>
-      <c r="C122" s="13"/>
-      <c r="D122" s="13"/>
-      <c r="E122" s="13"/>
-      <c r="F122" s="13"/>
-      <c r="G122" s="13"/>
-      <c r="H122" s="13"/>
-      <c r="I122" s="13"/>
-      <c r="J122" s="13"/>
-      <c r="K122" s="13"/>
-      <c r="L122" s="13"/>
-      <c r="M122" s="13"/>
-      <c r="N122" s="13"/>
-      <c r="O122" s="13"/>
-      <c r="P122" s="13"/>
-      <c r="Q122" s="13"/>
-      <c r="R122" s="13"/>
       <c r="S122" s="6"/>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
-      <c r="B123" s="13"/>
-      <c r="C123" s="13"/>
-      <c r="D123" s="13"/>
-      <c r="E123" s="13"/>
-      <c r="F123" s="13"/>
-      <c r="G123" s="13"/>
-      <c r="H123" s="13"/>
-      <c r="I123" s="13"/>
-      <c r="J123" s="13"/>
-      <c r="K123" s="13"/>
-      <c r="L123" s="13"/>
-      <c r="M123" s="13"/>
-      <c r="N123" s="13"/>
-      <c r="O123" s="13"/>
-      <c r="P123" s="13"/>
-      <c r="Q123" s="13"/>
-      <c r="R123" s="13"/>
       <c r="S123" s="6"/>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
-      <c r="B124" s="13"/>
-      <c r="C124" s="13"/>
-      <c r="D124" s="13"/>
-      <c r="E124" s="13"/>
-      <c r="F124" s="13"/>
-      <c r="G124" s="13"/>
-      <c r="H124" s="13"/>
-      <c r="I124" s="13"/>
-      <c r="J124" s="13"/>
-      <c r="K124" s="13"/>
-      <c r="L124" s="13"/>
-      <c r="M124" s="13"/>
-      <c r="N124" s="13"/>
-      <c r="O124" s="13"/>
-      <c r="P124" s="13"/>
-      <c r="Q124" s="13"/>
-      <c r="R124" s="13"/>
       <c r="S124" s="6"/>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
-      <c r="B125" s="13"/>
-      <c r="C125" s="13"/>
-      <c r="D125" s="13"/>
-      <c r="E125" s="13"/>
-      <c r="F125" s="13"/>
-      <c r="G125" s="13"/>
-      <c r="H125" s="13"/>
-      <c r="I125" s="13"/>
-      <c r="J125" s="13"/>
-      <c r="K125" s="13"/>
-      <c r="L125" s="13"/>
-      <c r="M125" s="13"/>
-      <c r="N125" s="13"/>
-      <c r="O125" s="13"/>
-      <c r="P125" s="13"/>
-      <c r="Q125" s="13"/>
-      <c r="R125" s="13"/>
       <c r="S125" s="6"/>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
-      <c r="B126" s="13"/>
-      <c r="C126" s="13"/>
-      <c r="D126" s="13"/>
-      <c r="E126" s="13"/>
-      <c r="F126" s="13"/>
-      <c r="G126" s="13"/>
-      <c r="H126" s="13"/>
-      <c r="I126" s="13"/>
-      <c r="J126" s="13"/>
-      <c r="K126" s="13"/>
-      <c r="L126" s="13"/>
-      <c r="M126" s="13"/>
-      <c r="N126" s="13"/>
-      <c r="O126" s="13"/>
-      <c r="P126" s="13"/>
-      <c r="Q126" s="13"/>
-      <c r="R126" s="13"/>
       <c r="S126" s="6"/>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
-      <c r="B127" s="13"/>
-      <c r="C127" s="13"/>
-      <c r="D127" s="13"/>
-      <c r="E127" s="13"/>
-      <c r="F127" s="13"/>
-      <c r="G127" s="13"/>
-      <c r="H127" s="13"/>
-      <c r="I127" s="13"/>
-      <c r="J127" s="13"/>
-      <c r="K127" s="13"/>
-      <c r="L127" s="13"/>
-      <c r="M127" s="13"/>
-      <c r="N127" s="13"/>
-      <c r="O127" s="13"/>
-      <c r="P127" s="13"/>
-      <c r="Q127" s="13"/>
-      <c r="R127" s="13"/>
       <c r="S127" s="6"/>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
-      <c r="B128" s="13"/>
-      <c r="C128" s="13"/>
-      <c r="D128" s="13"/>
-      <c r="E128" s="13"/>
-      <c r="F128" s="13"/>
-      <c r="G128" s="13"/>
-      <c r="H128" s="13"/>
-      <c r="I128" s="13"/>
-      <c r="J128" s="13"/>
-      <c r="K128" s="13"/>
-      <c r="L128" s="13"/>
-      <c r="M128" s="13"/>
-      <c r="N128" s="13"/>
-      <c r="O128" s="13"/>
-      <c r="P128" s="13"/>
-      <c r="Q128" s="13"/>
-      <c r="R128" s="13"/>
       <c r="S128" s="6"/>
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
-      <c r="B129" s="13"/>
-      <c r="C129" s="13"/>
-      <c r="D129" s="13"/>
-      <c r="E129" s="13"/>
-      <c r="F129" s="13"/>
-      <c r="G129" s="13"/>
-      <c r="H129" s="13"/>
-      <c r="I129" s="13"/>
-      <c r="J129" s="13"/>
-      <c r="K129" s="13"/>
-      <c r="L129" s="13"/>
-      <c r="M129" s="13"/>
-      <c r="N129" s="13"/>
-      <c r="O129" s="13"/>
-      <c r="P129" s="13"/>
-      <c r="Q129" s="13"/>
-      <c r="R129" s="13"/>
       <c r="S129" s="6"/>
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
-      <c r="B130" s="13"/>
-      <c r="C130" s="13"/>
-      <c r="D130" s="13"/>
-      <c r="E130" s="13"/>
-      <c r="F130" s="13"/>
-      <c r="G130" s="13"/>
-      <c r="H130" s="13"/>
-      <c r="I130" s="13"/>
-      <c r="J130" s="13"/>
-      <c r="K130" s="13"/>
-      <c r="L130" s="13"/>
-      <c r="M130" s="13"/>
-      <c r="N130" s="13"/>
-      <c r="O130" s="13"/>
-      <c r="P130" s="13"/>
-      <c r="Q130" s="13"/>
-      <c r="R130" s="13"/>
       <c r="S130" s="6"/>
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
-      <c r="B131" s="13"/>
-      <c r="C131" s="13"/>
-      <c r="D131" s="13"/>
-      <c r="E131" s="13"/>
-      <c r="F131" s="13"/>
-      <c r="G131" s="13"/>
-      <c r="H131" s="13"/>
-      <c r="I131" s="13"/>
-      <c r="J131" s="13"/>
-      <c r="K131" s="13"/>
-      <c r="L131" s="13"/>
-      <c r="M131" s="13"/>
-      <c r="N131" s="13"/>
-      <c r="O131" s="13"/>
-      <c r="P131" s="13"/>
-      <c r="Q131" s="13"/>
-      <c r="R131" s="13"/>
       <c r="S131" s="6"/>
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
-      <c r="B132" s="13"/>
-      <c r="C132" s="13"/>
-      <c r="D132" s="13"/>
-      <c r="E132" s="13"/>
-      <c r="F132" s="13"/>
-      <c r="G132" s="13"/>
-      <c r="H132" s="13"/>
-      <c r="I132" s="13"/>
-      <c r="J132" s="13"/>
-      <c r="K132" s="13"/>
-      <c r="L132" s="13"/>
-      <c r="M132" s="13"/>
-      <c r="N132" s="13"/>
-      <c r="O132" s="13"/>
-      <c r="P132" s="13"/>
-      <c r="Q132" s="13"/>
-      <c r="R132" s="13"/>
       <c r="S132" s="6"/>
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
-      <c r="B133" s="13"/>
-      <c r="C133" s="13"/>
-      <c r="D133" s="13"/>
-      <c r="E133" s="13"/>
-      <c r="F133" s="13"/>
-      <c r="G133" s="13"/>
-      <c r="H133" s="13"/>
-      <c r="I133" s="13"/>
-      <c r="J133" s="13"/>
-      <c r="K133" s="13"/>
-      <c r="L133" s="13"/>
-      <c r="M133" s="13"/>
-      <c r="N133" s="13"/>
-      <c r="O133" s="13"/>
-      <c r="P133" s="13"/>
-      <c r="Q133" s="13"/>
-      <c r="R133" s="13"/>
       <c r="S133" s="6"/>
     </row>
     <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
-      <c r="B134" s="13"/>
-      <c r="C134" s="13"/>
-      <c r="D134" s="13"/>
-      <c r="E134" s="13"/>
-      <c r="F134" s="13"/>
-      <c r="G134" s="13"/>
-      <c r="H134" s="13"/>
-      <c r="I134" s="13"/>
-      <c r="J134" s="13"/>
-      <c r="K134" s="13"/>
-      <c r="L134" s="13"/>
-      <c r="M134" s="13"/>
-      <c r="N134" s="13"/>
-      <c r="O134" s="13"/>
-      <c r="P134" s="13"/>
-      <c r="Q134" s="13"/>
-      <c r="R134" s="13"/>
       <c r="S134" s="6"/>
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.25">
@@ -7609,15 +6187,6 @@
       <c r="H139" s="3"/>
       <c r="I139" s="3"/>
       <c r="J139" s="4"/>
-      <c r="K139" s="13"/>
-      <c r="L139" s="13"/>
-      <c r="M139" s="13"/>
-      <c r="N139" s="13"/>
-      <c r="O139" s="13"/>
-      <c r="P139" s="13"/>
-      <c r="Q139" s="13"/>
-      <c r="R139" s="13"/>
-      <c r="S139" s="13"/>
       <c r="T139" s="6"/>
     </row>
     <row r="140" spans="1:20" x14ac:dyDescent="0.25">
@@ -7625,23 +6194,7 @@
       <c r="B140" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C140" s="13"/>
-      <c r="D140" s="13"/>
-      <c r="E140" s="13"/>
-      <c r="F140" s="13"/>
-      <c r="G140" s="13"/>
-      <c r="H140" s="13"/>
-      <c r="I140" s="13"/>
       <c r="J140" s="6"/>
-      <c r="K140" s="13"/>
-      <c r="L140" s="13"/>
-      <c r="M140" s="13"/>
-      <c r="N140" s="13"/>
-      <c r="O140" s="13"/>
-      <c r="P140" s="13"/>
-      <c r="Q140" s="13"/>
-      <c r="R140" s="13"/>
-      <c r="S140" s="13"/>
       <c r="T140" s="6"/>
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.25">
@@ -7649,23 +6202,7 @@
       <c r="B141" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C141" s="13"/>
-      <c r="D141" s="13"/>
-      <c r="E141" s="13"/>
-      <c r="F141" s="13"/>
-      <c r="G141" s="13"/>
-      <c r="H141" s="13"/>
-      <c r="I141" s="13"/>
       <c r="J141" s="6"/>
-      <c r="K141" s="13"/>
-      <c r="L141" s="13"/>
-      <c r="M141" s="13"/>
-      <c r="N141" s="13"/>
-      <c r="O141" s="13"/>
-      <c r="P141" s="13"/>
-      <c r="Q141" s="13"/>
-      <c r="R141" s="13"/>
-      <c r="S141" s="13"/>
       <c r="T141" s="6"/>
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.25">
@@ -7673,23 +6210,7 @@
       <c r="B142" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C142" s="13"/>
-      <c r="D142" s="13"/>
-      <c r="E142" s="13"/>
-      <c r="F142" s="13"/>
-      <c r="G142" s="13"/>
-      <c r="H142" s="13"/>
-      <c r="I142" s="13"/>
       <c r="J142" s="6"/>
-      <c r="K142" s="13"/>
-      <c r="L142" s="13"/>
-      <c r="M142" s="13"/>
-      <c r="N142" s="13"/>
-      <c r="O142" s="13"/>
-      <c r="P142" s="13"/>
-      <c r="Q142" s="13"/>
-      <c r="R142" s="13"/>
-      <c r="S142" s="13"/>
       <c r="T142" s="6"/>
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.25">
@@ -7697,23 +6218,7 @@
       <c r="B143" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C143" s="13"/>
-      <c r="D143" s="13"/>
-      <c r="E143" s="13"/>
-      <c r="F143" s="13"/>
-      <c r="G143" s="13"/>
-      <c r="H143" s="13"/>
-      <c r="I143" s="13"/>
       <c r="J143" s="6"/>
-      <c r="K143" s="13"/>
-      <c r="L143" s="13"/>
-      <c r="M143" s="13"/>
-      <c r="N143" s="13"/>
-      <c r="O143" s="13"/>
-      <c r="P143" s="13"/>
-      <c r="Q143" s="13"/>
-      <c r="R143" s="13"/>
-      <c r="S143" s="13"/>
       <c r="T143" s="6"/>
     </row>
     <row r="144" spans="1:20" x14ac:dyDescent="0.25">
@@ -7721,23 +6226,7 @@
       <c r="B144" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C144" s="13"/>
-      <c r="D144" s="13"/>
-      <c r="E144" s="13"/>
-      <c r="F144" s="13"/>
-      <c r="G144" s="13"/>
-      <c r="H144" s="13"/>
-      <c r="I144" s="13"/>
       <c r="J144" s="6"/>
-      <c r="K144" s="13"/>
-      <c r="L144" s="13"/>
-      <c r="M144" s="13"/>
-      <c r="N144" s="13"/>
-      <c r="O144" s="13"/>
-      <c r="P144" s="13"/>
-      <c r="Q144" s="13"/>
-      <c r="R144" s="13"/>
-      <c r="S144" s="13"/>
       <c r="T144" s="6"/>
     </row>
     <row r="145" spans="1:20" x14ac:dyDescent="0.25">
@@ -7745,23 +6234,7 @@
       <c r="B145" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C145" s="13"/>
-      <c r="D145" s="13"/>
-      <c r="E145" s="13"/>
-      <c r="F145" s="13"/>
-      <c r="G145" s="13"/>
-      <c r="H145" s="13"/>
-      <c r="I145" s="13"/>
       <c r="J145" s="6"/>
-      <c r="K145" s="13"/>
-      <c r="L145" s="13"/>
-      <c r="M145" s="13"/>
-      <c r="N145" s="13"/>
-      <c r="O145" s="13"/>
-      <c r="P145" s="13"/>
-      <c r="Q145" s="13"/>
-      <c r="R145" s="13"/>
-      <c r="S145" s="13"/>
       <c r="T145" s="6"/>
     </row>
     <row r="146" spans="1:20" x14ac:dyDescent="0.25">
@@ -7769,23 +6242,7 @@
       <c r="B146" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C146" s="13"/>
-      <c r="D146" s="13"/>
-      <c r="E146" s="13"/>
-      <c r="F146" s="13"/>
-      <c r="G146" s="13"/>
-      <c r="H146" s="13"/>
-      <c r="I146" s="13"/>
       <c r="J146" s="6"/>
-      <c r="K146" s="13"/>
-      <c r="L146" s="13"/>
-      <c r="M146" s="13"/>
-      <c r="N146" s="13"/>
-      <c r="O146" s="13"/>
-      <c r="P146" s="13"/>
-      <c r="Q146" s="13"/>
-      <c r="R146" s="13"/>
-      <c r="S146" s="13"/>
       <c r="T146" s="6"/>
     </row>
     <row r="147" spans="1:20" x14ac:dyDescent="0.25">
@@ -7793,23 +6250,7 @@
       <c r="B147" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C147" s="13"/>
-      <c r="D147" s="13"/>
-      <c r="E147" s="13"/>
-      <c r="F147" s="13"/>
-      <c r="G147" s="13"/>
-      <c r="H147" s="13"/>
-      <c r="I147" s="13"/>
       <c r="J147" s="6"/>
-      <c r="K147" s="13"/>
-      <c r="L147" s="13"/>
-      <c r="M147" s="13"/>
-      <c r="N147" s="13"/>
-      <c r="O147" s="13"/>
-      <c r="P147" s="13"/>
-      <c r="Q147" s="13"/>
-      <c r="R147" s="13"/>
-      <c r="S147" s="13"/>
       <c r="T147" s="6"/>
     </row>
     <row r="148" spans="1:20" x14ac:dyDescent="0.25">
@@ -7817,23 +6258,7 @@
       <c r="B148" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C148" s="13"/>
-      <c r="D148" s="13"/>
-      <c r="E148" s="13"/>
-      <c r="F148" s="13"/>
-      <c r="G148" s="13"/>
-      <c r="H148" s="13"/>
-      <c r="I148" s="13"/>
       <c r="J148" s="6"/>
-      <c r="K148" s="13"/>
-      <c r="L148" s="13"/>
-      <c r="M148" s="13"/>
-      <c r="N148" s="13"/>
-      <c r="O148" s="13"/>
-      <c r="P148" s="13"/>
-      <c r="Q148" s="13"/>
-      <c r="R148" s="13"/>
-      <c r="S148" s="13"/>
       <c r="T148" s="6"/>
     </row>
     <row r="149" spans="1:20" x14ac:dyDescent="0.25">
@@ -7841,23 +6266,7 @@
       <c r="B149" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C149" s="13"/>
-      <c r="D149" s="13"/>
-      <c r="E149" s="13"/>
-      <c r="F149" s="13"/>
-      <c r="G149" s="13"/>
-      <c r="H149" s="13"/>
-      <c r="I149" s="13"/>
       <c r="J149" s="6"/>
-      <c r="K149" s="13"/>
-      <c r="L149" s="13"/>
-      <c r="M149" s="13"/>
-      <c r="N149" s="13"/>
-      <c r="O149" s="13"/>
-      <c r="P149" s="13"/>
-      <c r="Q149" s="13"/>
-      <c r="R149" s="13"/>
-      <c r="S149" s="13"/>
       <c r="T149" s="6"/>
     </row>
     <row r="150" spans="1:20" x14ac:dyDescent="0.25">
@@ -7865,23 +6274,7 @@
       <c r="B150" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C150" s="13"/>
-      <c r="D150" s="13"/>
-      <c r="E150" s="13"/>
-      <c r="F150" s="13"/>
-      <c r="G150" s="13"/>
-      <c r="H150" s="13"/>
-      <c r="I150" s="13"/>
       <c r="J150" s="6"/>
-      <c r="K150" s="13"/>
-      <c r="L150" s="13"/>
-      <c r="M150" s="13"/>
-      <c r="N150" s="13"/>
-      <c r="O150" s="13"/>
-      <c r="P150" s="13"/>
-      <c r="Q150" s="13"/>
-      <c r="R150" s="13"/>
-      <c r="S150" s="13"/>
       <c r="T150" s="6"/>
     </row>
     <row r="151" spans="1:20" x14ac:dyDescent="0.25">
@@ -7889,23 +6282,7 @@
       <c r="B151" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C151" s="13"/>
-      <c r="D151" s="13"/>
-      <c r="E151" s="13"/>
-      <c r="F151" s="13"/>
-      <c r="G151" s="13"/>
-      <c r="H151" s="13"/>
-      <c r="I151" s="13"/>
       <c r="J151" s="6"/>
-      <c r="K151" s="13"/>
-      <c r="L151" s="13"/>
-      <c r="M151" s="13"/>
-      <c r="N151" s="13"/>
-      <c r="O151" s="13"/>
-      <c r="P151" s="13"/>
-      <c r="Q151" s="13"/>
-      <c r="R151" s="13"/>
-      <c r="S151" s="13"/>
       <c r="T151" s="6"/>
     </row>
     <row r="152" spans="1:20" x14ac:dyDescent="0.25">
@@ -7913,23 +6290,7 @@
       <c r="B152" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C152" s="13"/>
-      <c r="D152" s="13"/>
-      <c r="E152" s="13"/>
-      <c r="F152" s="13"/>
-      <c r="G152" s="13"/>
-      <c r="H152" s="13"/>
-      <c r="I152" s="13"/>
       <c r="J152" s="6"/>
-      <c r="K152" s="13"/>
-      <c r="L152" s="13"/>
-      <c r="M152" s="13"/>
-      <c r="N152" s="13"/>
-      <c r="O152" s="13"/>
-      <c r="P152" s="13"/>
-      <c r="Q152" s="13"/>
-      <c r="R152" s="13"/>
-      <c r="S152" s="13"/>
       <c r="T152" s="6"/>
     </row>
     <row r="153" spans="1:20" x14ac:dyDescent="0.25">
@@ -7937,23 +6298,7 @@
       <c r="B153" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C153" s="13"/>
-      <c r="D153" s="13"/>
-      <c r="E153" s="13"/>
-      <c r="F153" s="13"/>
-      <c r="G153" s="13"/>
-      <c r="H153" s="13"/>
-      <c r="I153" s="13"/>
       <c r="J153" s="6"/>
-      <c r="K153" s="13"/>
-      <c r="L153" s="13"/>
-      <c r="M153" s="13"/>
-      <c r="N153" s="13"/>
-      <c r="O153" s="13"/>
-      <c r="P153" s="13"/>
-      <c r="Q153" s="13"/>
-      <c r="R153" s="13"/>
-      <c r="S153" s="13"/>
       <c r="T153" s="6"/>
     </row>
     <row r="154" spans="1:20" x14ac:dyDescent="0.25">
@@ -7961,23 +6306,7 @@
       <c r="B154" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C154" s="13"/>
-      <c r="D154" s="13"/>
-      <c r="E154" s="13"/>
-      <c r="F154" s="13"/>
-      <c r="G154" s="13"/>
-      <c r="H154" s="13"/>
-      <c r="I154" s="13"/>
       <c r="J154" s="6"/>
-      <c r="K154" s="13"/>
-      <c r="L154" s="13"/>
-      <c r="M154" s="13"/>
-      <c r="N154" s="13"/>
-      <c r="O154" s="13"/>
-      <c r="P154" s="13"/>
-      <c r="Q154" s="13"/>
-      <c r="R154" s="13"/>
-      <c r="S154" s="13"/>
       <c r="T154" s="6"/>
     </row>
     <row r="155" spans="1:20" x14ac:dyDescent="0.25">
@@ -7985,23 +6314,7 @@
       <c r="B155" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C155" s="13"/>
-      <c r="D155" s="13"/>
-      <c r="E155" s="13"/>
-      <c r="F155" s="13"/>
-      <c r="G155" s="13"/>
-      <c r="H155" s="13"/>
-      <c r="I155" s="13"/>
       <c r="J155" s="6"/>
-      <c r="K155" s="13"/>
-      <c r="L155" s="13"/>
-      <c r="M155" s="13"/>
-      <c r="N155" s="13"/>
-      <c r="O155" s="13"/>
-      <c r="P155" s="13"/>
-      <c r="Q155" s="13"/>
-      <c r="R155" s="13"/>
-      <c r="S155" s="13"/>
       <c r="T155" s="6"/>
     </row>
     <row r="156" spans="1:20" x14ac:dyDescent="0.25">
@@ -8009,23 +6322,7 @@
       <c r="B156" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C156" s="13"/>
-      <c r="D156" s="13"/>
-      <c r="E156" s="13"/>
-      <c r="F156" s="13"/>
-      <c r="G156" s="13"/>
-      <c r="H156" s="13"/>
-      <c r="I156" s="13"/>
       <c r="J156" s="6"/>
-      <c r="K156" s="13"/>
-      <c r="L156" s="13"/>
-      <c r="M156" s="13"/>
-      <c r="N156" s="13"/>
-      <c r="O156" s="13"/>
-      <c r="P156" s="13"/>
-      <c r="Q156" s="13"/>
-      <c r="R156" s="13"/>
-      <c r="S156" s="13"/>
       <c r="T156" s="6"/>
     </row>
     <row r="157" spans="1:20" x14ac:dyDescent="0.25">
@@ -8033,23 +6330,7 @@
       <c r="B157" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C157" s="13"/>
-      <c r="D157" s="13"/>
-      <c r="E157" s="13"/>
-      <c r="F157" s="13"/>
-      <c r="G157" s="13"/>
-      <c r="H157" s="13"/>
-      <c r="I157" s="13"/>
       <c r="J157" s="6"/>
-      <c r="K157" s="13"/>
-      <c r="L157" s="13"/>
-      <c r="M157" s="13"/>
-      <c r="N157" s="13"/>
-      <c r="O157" s="13"/>
-      <c r="P157" s="13"/>
-      <c r="Q157" s="13"/>
-      <c r="R157" s="13"/>
-      <c r="S157" s="13"/>
       <c r="T157" s="6"/>
     </row>
     <row r="158" spans="1:20" x14ac:dyDescent="0.25">
@@ -8065,59 +6346,14 @@
       <c r="H158" s="9"/>
       <c r="I158" s="9"/>
       <c r="J158" s="10"/>
-      <c r="K158" s="13"/>
-      <c r="L158" s="13"/>
-      <c r="M158" s="13"/>
-      <c r="N158" s="13"/>
-      <c r="O158" s="13"/>
-      <c r="P158" s="13"/>
-      <c r="Q158" s="13"/>
-      <c r="R158" s="13"/>
-      <c r="S158" s="13"/>
       <c r="T158" s="6"/>
     </row>
     <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
-      <c r="B159" s="13"/>
-      <c r="C159" s="13"/>
-      <c r="D159" s="13"/>
-      <c r="E159" s="13"/>
-      <c r="F159" s="13"/>
-      <c r="G159" s="13"/>
-      <c r="H159" s="13"/>
-      <c r="I159" s="13"/>
-      <c r="J159" s="13"/>
-      <c r="K159" s="13"/>
-      <c r="L159" s="13"/>
-      <c r="M159" s="13"/>
-      <c r="N159" s="13"/>
-      <c r="O159" s="13"/>
-      <c r="P159" s="13"/>
-      <c r="Q159" s="13"/>
-      <c r="R159" s="13"/>
-      <c r="S159" s="13"/>
       <c r="T159" s="6"/>
     </row>
     <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" s="5"/>
-      <c r="B160" s="13"/>
-      <c r="C160" s="13"/>
-      <c r="D160" s="13"/>
-      <c r="E160" s="13"/>
-      <c r="F160" s="13"/>
-      <c r="G160" s="13"/>
-      <c r="H160" s="13"/>
-      <c r="I160" s="13"/>
-      <c r="J160" s="13"/>
-      <c r="K160" s="13"/>
-      <c r="L160" s="13"/>
-      <c r="M160" s="13"/>
-      <c r="N160" s="13"/>
-      <c r="O160" s="13"/>
-      <c r="P160" s="13"/>
-      <c r="Q160" s="13"/>
-      <c r="R160" s="13"/>
-      <c r="S160" s="13"/>
       <c r="T160" s="6"/>
     </row>
     <row r="161" spans="1:20" x14ac:dyDescent="0.25">
@@ -8147,638 +6383,174 @@
     <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
       <c r="B162" s="5"/>
-      <c r="C162" s="13"/>
-      <c r="D162" s="13"/>
-      <c r="E162" s="13"/>
-      <c r="F162" s="13"/>
-      <c r="G162" s="13"/>
-      <c r="H162" s="13"/>
-      <c r="I162" s="13"/>
-      <c r="J162" s="13"/>
-      <c r="K162" s="13"/>
-      <c r="L162" s="13"/>
-      <c r="M162" s="13"/>
-      <c r="N162" s="13"/>
-      <c r="O162" s="13"/>
-      <c r="P162" s="13"/>
-      <c r="Q162" s="13"/>
-      <c r="R162" s="13"/>
       <c r="S162" s="6"/>
       <c r="T162" s="6"/>
     </row>
     <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
       <c r="B163" s="5"/>
-      <c r="C163" s="13"/>
-      <c r="D163" s="13"/>
-      <c r="E163" s="13"/>
-      <c r="F163" s="13"/>
-      <c r="G163" s="13"/>
-      <c r="H163" s="13"/>
-      <c r="I163" s="13"/>
-      <c r="J163" s="13"/>
-      <c r="K163" s="13"/>
-      <c r="L163" s="13"/>
-      <c r="M163" s="13"/>
-      <c r="N163" s="13"/>
-      <c r="O163" s="13"/>
-      <c r="P163" s="13"/>
-      <c r="Q163" s="13"/>
-      <c r="R163" s="13"/>
       <c r="S163" s="6"/>
       <c r="T163" s="6"/>
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
       <c r="B164" s="5"/>
-      <c r="C164" s="13"/>
-      <c r="D164" s="13"/>
-      <c r="E164" s="13"/>
-      <c r="F164" s="13"/>
-      <c r="G164" s="13"/>
-      <c r="H164" s="13"/>
-      <c r="I164" s="13"/>
-      <c r="J164" s="13"/>
-      <c r="K164" s="13"/>
-      <c r="L164" s="13"/>
-      <c r="M164" s="13"/>
-      <c r="N164" s="13"/>
-      <c r="O164" s="13"/>
-      <c r="P164" s="13"/>
-      <c r="Q164" s="13"/>
-      <c r="R164" s="13"/>
       <c r="S164" s="6"/>
       <c r="T164" s="6"/>
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
       <c r="B165" s="5"/>
-      <c r="C165" s="13"/>
-      <c r="D165" s="13"/>
-      <c r="E165" s="13"/>
-      <c r="F165" s="13"/>
-      <c r="G165" s="13"/>
-      <c r="H165" s="13"/>
-      <c r="I165" s="13"/>
-      <c r="J165" s="13"/>
-      <c r="K165" s="13"/>
-      <c r="L165" s="13"/>
-      <c r="M165" s="13"/>
-      <c r="N165" s="13"/>
-      <c r="O165" s="13"/>
-      <c r="P165" s="13"/>
-      <c r="Q165" s="13"/>
-      <c r="R165" s="13"/>
       <c r="S165" s="6"/>
       <c r="T165" s="6"/>
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" s="5"/>
       <c r="B166" s="5"/>
-      <c r="C166" s="13"/>
-      <c r="D166" s="13"/>
-      <c r="E166" s="13"/>
-      <c r="F166" s="13"/>
-      <c r="G166" s="13"/>
-      <c r="H166" s="13"/>
-      <c r="I166" s="13"/>
-      <c r="J166" s="13"/>
-      <c r="K166" s="13"/>
-      <c r="L166" s="13"/>
-      <c r="M166" s="13"/>
-      <c r="N166" s="13"/>
-      <c r="O166" s="13"/>
-      <c r="P166" s="13"/>
-      <c r="Q166" s="13"/>
-      <c r="R166" s="13"/>
       <c r="S166" s="6"/>
       <c r="T166" s="6"/>
     </row>
     <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" s="5"/>
       <c r="B167" s="5"/>
-      <c r="C167" s="13"/>
-      <c r="D167" s="13"/>
-      <c r="E167" s="13"/>
-      <c r="F167" s="13"/>
-      <c r="G167" s="13"/>
-      <c r="H167" s="13"/>
-      <c r="I167" s="13"/>
-      <c r="J167" s="13"/>
-      <c r="K167" s="13"/>
-      <c r="L167" s="13"/>
-      <c r="M167" s="13"/>
-      <c r="N167" s="13"/>
-      <c r="O167" s="13"/>
-      <c r="P167" s="13"/>
-      <c r="Q167" s="13"/>
-      <c r="R167" s="13"/>
       <c r="S167" s="6"/>
       <c r="T167" s="6"/>
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>
       <c r="B168" s="5"/>
-      <c r="C168" s="13"/>
-      <c r="D168" s="13"/>
-      <c r="E168" s="13"/>
-      <c r="F168" s="13"/>
-      <c r="G168" s="13"/>
-      <c r="H168" s="13"/>
-      <c r="I168" s="13"/>
-      <c r="J168" s="13"/>
-      <c r="K168" s="13"/>
-      <c r="L168" s="13"/>
-      <c r="M168" s="13"/>
-      <c r="N168" s="13"/>
-      <c r="O168" s="13"/>
-      <c r="P168" s="13"/>
-      <c r="Q168" s="13"/>
-      <c r="R168" s="13"/>
       <c r="S168" s="6"/>
       <c r="T168" s="6"/>
     </row>
     <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>
       <c r="B169" s="5"/>
-      <c r="C169" s="13"/>
-      <c r="D169" s="13"/>
-      <c r="E169" s="13"/>
-      <c r="F169" s="13"/>
-      <c r="G169" s="13"/>
-      <c r="H169" s="13"/>
-      <c r="I169" s="13"/>
-      <c r="J169" s="13"/>
-      <c r="K169" s="13"/>
-      <c r="L169" s="13"/>
-      <c r="M169" s="13"/>
-      <c r="N169" s="13"/>
-      <c r="O169" s="13"/>
-      <c r="P169" s="13"/>
-      <c r="Q169" s="13"/>
-      <c r="R169" s="13"/>
       <c r="S169" s="6"/>
       <c r="T169" s="6"/>
     </row>
     <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" s="5"/>
       <c r="B170" s="5"/>
-      <c r="C170" s="13"/>
-      <c r="D170" s="13"/>
-      <c r="E170" s="13"/>
-      <c r="F170" s="13"/>
-      <c r="G170" s="13"/>
-      <c r="H170" s="13"/>
-      <c r="I170" s="13"/>
-      <c r="J170" s="13"/>
-      <c r="K170" s="13"/>
-      <c r="L170" s="13"/>
-      <c r="M170" s="13"/>
-      <c r="N170" s="13"/>
-      <c r="O170" s="13"/>
-      <c r="P170" s="13"/>
-      <c r="Q170" s="13"/>
-      <c r="R170" s="13"/>
       <c r="S170" s="6"/>
       <c r="T170" s="6"/>
     </row>
     <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
       <c r="B171" s="5"/>
-      <c r="C171" s="13"/>
-      <c r="D171" s="13"/>
-      <c r="E171" s="13"/>
-      <c r="F171" s="13"/>
-      <c r="G171" s="13"/>
-      <c r="H171" s="13"/>
-      <c r="I171" s="13"/>
-      <c r="J171" s="13"/>
-      <c r="K171" s="13"/>
-      <c r="L171" s="13"/>
-      <c r="M171" s="13"/>
-      <c r="N171" s="13"/>
-      <c r="O171" s="13"/>
-      <c r="P171" s="13"/>
-      <c r="Q171" s="13"/>
-      <c r="R171" s="13"/>
       <c r="S171" s="6"/>
       <c r="T171" s="6"/>
     </row>
     <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
       <c r="B172" s="5"/>
-      <c r="C172" s="13"/>
-      <c r="D172" s="13"/>
-      <c r="E172" s="13"/>
-      <c r="F172" s="13"/>
-      <c r="G172" s="13"/>
-      <c r="H172" s="13"/>
-      <c r="I172" s="13"/>
-      <c r="J172" s="13"/>
-      <c r="K172" s="13"/>
-      <c r="L172" s="13"/>
-      <c r="M172" s="13"/>
-      <c r="N172" s="13"/>
-      <c r="O172" s="13"/>
-      <c r="P172" s="13"/>
-      <c r="Q172" s="13"/>
-      <c r="R172" s="13"/>
       <c r="S172" s="6"/>
       <c r="T172" s="6"/>
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" s="5"/>
       <c r="B173" s="5"/>
-      <c r="C173" s="13"/>
-      <c r="D173" s="13"/>
-      <c r="E173" s="13"/>
-      <c r="F173" s="13"/>
-      <c r="G173" s="13"/>
-      <c r="H173" s="13"/>
-      <c r="I173" s="13"/>
-      <c r="J173" s="13"/>
-      <c r="K173" s="13"/>
-      <c r="L173" s="13"/>
-      <c r="M173" s="13"/>
-      <c r="N173" s="13"/>
-      <c r="O173" s="13"/>
-      <c r="P173" s="13"/>
-      <c r="Q173" s="13"/>
-      <c r="R173" s="13"/>
       <c r="S173" s="6"/>
       <c r="T173" s="6"/>
     </row>
     <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" s="5"/>
       <c r="B174" s="5"/>
-      <c r="C174" s="13"/>
-      <c r="D174" s="13"/>
-      <c r="E174" s="13"/>
-      <c r="F174" s="13"/>
-      <c r="G174" s="13"/>
-      <c r="H174" s="13"/>
-      <c r="I174" s="13"/>
-      <c r="J174" s="13"/>
-      <c r="K174" s="13"/>
-      <c r="L174" s="13"/>
-      <c r="M174" s="13"/>
-      <c r="N174" s="13"/>
-      <c r="O174" s="13"/>
-      <c r="P174" s="13"/>
-      <c r="Q174" s="13"/>
-      <c r="R174" s="13"/>
       <c r="S174" s="6"/>
       <c r="T174" s="6"/>
     </row>
     <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
       <c r="B175" s="5"/>
-      <c r="C175" s="13"/>
-      <c r="D175" s="13"/>
-      <c r="E175" s="13"/>
-      <c r="F175" s="13"/>
-      <c r="G175" s="13"/>
-      <c r="H175" s="13"/>
-      <c r="I175" s="13"/>
-      <c r="J175" s="13"/>
-      <c r="K175" s="13"/>
-      <c r="L175" s="13"/>
-      <c r="M175" s="13"/>
-      <c r="N175" s="13"/>
-      <c r="O175" s="13"/>
-      <c r="P175" s="13"/>
-      <c r="Q175" s="13"/>
-      <c r="R175" s="13"/>
       <c r="S175" s="6"/>
       <c r="T175" s="6"/>
     </row>
     <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
       <c r="B176" s="5"/>
-      <c r="C176" s="13"/>
-      <c r="D176" s="13"/>
-      <c r="E176" s="13"/>
-      <c r="F176" s="13"/>
-      <c r="G176" s="13"/>
-      <c r="H176" s="13"/>
-      <c r="I176" s="13"/>
-      <c r="J176" s="13"/>
-      <c r="K176" s="13"/>
-      <c r="L176" s="13"/>
-      <c r="M176" s="13"/>
-      <c r="N176" s="13"/>
-      <c r="O176" s="13"/>
-      <c r="P176" s="13"/>
-      <c r="Q176" s="13"/>
-      <c r="R176" s="13"/>
       <c r="S176" s="6"/>
       <c r="T176" s="6"/>
     </row>
     <row r="177" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A177" s="5"/>
       <c r="B177" s="5"/>
-      <c r="C177" s="13"/>
-      <c r="D177" s="13"/>
-      <c r="E177" s="13"/>
-      <c r="F177" s="13"/>
-      <c r="G177" s="13"/>
-      <c r="H177" s="13"/>
-      <c r="I177" s="13"/>
-      <c r="J177" s="13"/>
-      <c r="K177" s="13"/>
-      <c r="L177" s="13"/>
-      <c r="M177" s="13"/>
-      <c r="N177" s="13"/>
-      <c r="O177" s="13"/>
-      <c r="P177" s="13"/>
-      <c r="Q177" s="13"/>
-      <c r="R177" s="13"/>
       <c r="S177" s="6"/>
       <c r="T177" s="6"/>
     </row>
     <row r="178" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A178" s="5"/>
       <c r="B178" s="5"/>
-      <c r="C178" s="13"/>
-      <c r="D178" s="13"/>
-      <c r="E178" s="13"/>
-      <c r="F178" s="13"/>
-      <c r="G178" s="13"/>
-      <c r="H178" s="13"/>
-      <c r="I178" s="13"/>
-      <c r="J178" s="13"/>
-      <c r="K178" s="13"/>
-      <c r="L178" s="13"/>
-      <c r="M178" s="13"/>
-      <c r="N178" s="13"/>
-      <c r="O178" s="13"/>
-      <c r="P178" s="13"/>
-      <c r="Q178" s="13"/>
-      <c r="R178" s="13"/>
       <c r="S178" s="6"/>
       <c r="T178" s="6"/>
     </row>
     <row r="179" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A179" s="5"/>
       <c r="B179" s="5"/>
-      <c r="C179" s="13"/>
-      <c r="D179" s="13"/>
-      <c r="E179" s="13"/>
-      <c r="F179" s="13"/>
-      <c r="G179" s="13"/>
-      <c r="H179" s="13"/>
-      <c r="I179" s="13"/>
-      <c r="J179" s="13"/>
-      <c r="K179" s="13"/>
-      <c r="L179" s="13"/>
-      <c r="M179" s="13"/>
-      <c r="N179" s="13"/>
-      <c r="O179" s="13"/>
-      <c r="P179" s="13"/>
-      <c r="Q179" s="13"/>
-      <c r="R179" s="13"/>
       <c r="S179" s="6"/>
       <c r="T179" s="6"/>
     </row>
     <row r="180" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A180" s="5"/>
       <c r="B180" s="5"/>
-      <c r="C180" s="13"/>
-      <c r="D180" s="13"/>
-      <c r="E180" s="13"/>
-      <c r="F180" s="13"/>
-      <c r="G180" s="13"/>
-      <c r="H180" s="13"/>
-      <c r="I180" s="13"/>
-      <c r="J180" s="13"/>
-      <c r="K180" s="13"/>
-      <c r="L180" s="13"/>
-      <c r="M180" s="13"/>
-      <c r="N180" s="13"/>
-      <c r="O180" s="13"/>
-      <c r="P180" s="13"/>
-      <c r="Q180" s="13"/>
-      <c r="R180" s="13"/>
       <c r="S180" s="6"/>
       <c r="T180" s="6"/>
     </row>
     <row r="181" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A181" s="5"/>
       <c r="B181" s="5"/>
-      <c r="C181" s="13"/>
-      <c r="D181" s="13"/>
-      <c r="E181" s="13"/>
-      <c r="F181" s="13"/>
-      <c r="G181" s="13"/>
-      <c r="H181" s="13"/>
-      <c r="I181" s="13"/>
-      <c r="J181" s="13"/>
-      <c r="K181" s="13"/>
-      <c r="L181" s="13"/>
-      <c r="M181" s="13"/>
-      <c r="N181" s="13"/>
-      <c r="O181" s="13"/>
-      <c r="P181" s="13"/>
-      <c r="Q181" s="13"/>
-      <c r="R181" s="13"/>
       <c r="S181" s="6"/>
       <c r="T181" s="6"/>
     </row>
     <row r="182" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A182" s="5"/>
       <c r="B182" s="5"/>
-      <c r="C182" s="13"/>
-      <c r="D182" s="13"/>
-      <c r="E182" s="13"/>
-      <c r="F182" s="13"/>
-      <c r="G182" s="13"/>
-      <c r="H182" s="13"/>
-      <c r="I182" s="13"/>
-      <c r="J182" s="13"/>
-      <c r="K182" s="13"/>
-      <c r="L182" s="13"/>
-      <c r="M182" s="13"/>
-      <c r="N182" s="13"/>
-      <c r="O182" s="13"/>
-      <c r="P182" s="13"/>
-      <c r="Q182" s="13"/>
-      <c r="R182" s="13"/>
       <c r="S182" s="6"/>
       <c r="T182" s="6"/>
     </row>
     <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A183" s="5"/>
       <c r="B183" s="5"/>
-      <c r="C183" s="13"/>
-      <c r="D183" s="13"/>
-      <c r="E183" s="13"/>
-      <c r="F183" s="13"/>
-      <c r="G183" s="13"/>
-      <c r="H183" s="13"/>
-      <c r="I183" s="13"/>
-      <c r="J183" s="13"/>
-      <c r="K183" s="13"/>
-      <c r="L183" s="13"/>
-      <c r="M183" s="13"/>
-      <c r="N183" s="13"/>
-      <c r="O183" s="13"/>
-      <c r="P183" s="13"/>
-      <c r="Q183" s="13"/>
-      <c r="R183" s="13"/>
       <c r="S183" s="6"/>
       <c r="T183" s="6"/>
     </row>
     <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A184" s="5"/>
       <c r="B184" s="5"/>
-      <c r="C184" s="13"/>
-      <c r="D184" s="13"/>
-      <c r="E184" s="13"/>
-      <c r="F184" s="13"/>
-      <c r="G184" s="13"/>
-      <c r="H184" s="13"/>
-      <c r="I184" s="13"/>
-      <c r="J184" s="13"/>
-      <c r="K184" s="13"/>
-      <c r="L184" s="13"/>
-      <c r="M184" s="13"/>
-      <c r="N184" s="13"/>
-      <c r="O184" s="13"/>
-      <c r="P184" s="13"/>
-      <c r="Q184" s="13"/>
-      <c r="R184" s="13"/>
       <c r="S184" s="6"/>
       <c r="T184" s="6"/>
     </row>
     <row r="185" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A185" s="5"/>
       <c r="B185" s="5"/>
-      <c r="C185" s="13"/>
-      <c r="D185" s="13"/>
-      <c r="E185" s="13"/>
-      <c r="F185" s="13"/>
-      <c r="G185" s="13"/>
-      <c r="H185" s="13"/>
-      <c r="I185" s="13"/>
-      <c r="J185" s="13"/>
-      <c r="K185" s="13"/>
-      <c r="L185" s="13"/>
-      <c r="M185" s="13"/>
-      <c r="N185" s="13"/>
-      <c r="O185" s="13"/>
-      <c r="P185" s="13"/>
-      <c r="Q185" s="13"/>
-      <c r="R185" s="13"/>
       <c r="S185" s="6"/>
       <c r="T185" s="6"/>
     </row>
     <row r="186" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A186" s="5"/>
       <c r="B186" s="5"/>
-      <c r="C186" s="13"/>
-      <c r="D186" s="13"/>
-      <c r="E186" s="13"/>
-      <c r="F186" s="13"/>
-      <c r="G186" s="13"/>
-      <c r="H186" s="13"/>
-      <c r="I186" s="13"/>
-      <c r="J186" s="13"/>
-      <c r="K186" s="13"/>
-      <c r="L186" s="13"/>
-      <c r="M186" s="13"/>
-      <c r="N186" s="13"/>
-      <c r="O186" s="13"/>
-      <c r="P186" s="13"/>
-      <c r="Q186" s="13"/>
-      <c r="R186" s="13"/>
       <c r="S186" s="6"/>
       <c r="T186" s="6"/>
     </row>
     <row r="187" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A187" s="5"/>
       <c r="B187" s="5"/>
-      <c r="C187" s="13"/>
-      <c r="D187" s="13"/>
-      <c r="E187" s="13"/>
-      <c r="F187" s="13"/>
-      <c r="G187" s="13"/>
-      <c r="H187" s="13"/>
-      <c r="I187" s="13"/>
-      <c r="J187" s="13"/>
-      <c r="K187" s="13"/>
-      <c r="L187" s="13"/>
-      <c r="M187" s="13"/>
-      <c r="N187" s="13"/>
-      <c r="O187" s="13"/>
-      <c r="P187" s="13"/>
-      <c r="Q187" s="13"/>
-      <c r="R187" s="13"/>
       <c r="S187" s="6"/>
       <c r="T187" s="6"/>
     </row>
     <row r="188" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A188" s="5"/>
       <c r="B188" s="5"/>
-      <c r="C188" s="13"/>
-      <c r="D188" s="13"/>
-      <c r="E188" s="13"/>
-      <c r="F188" s="13"/>
-      <c r="G188" s="13"/>
-      <c r="H188" s="13"/>
-      <c r="I188" s="13"/>
-      <c r="J188" s="13"/>
-      <c r="K188" s="13"/>
-      <c r="L188" s="13"/>
-      <c r="M188" s="13"/>
-      <c r="N188" s="13"/>
-      <c r="O188" s="13"/>
-      <c r="P188" s="13"/>
-      <c r="Q188" s="13"/>
-      <c r="R188" s="13"/>
       <c r="S188" s="6"/>
       <c r="T188" s="6"/>
     </row>
     <row r="189" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A189" s="5"/>
       <c r="B189" s="5"/>
-      <c r="C189" s="13"/>
-      <c r="D189" s="13"/>
-      <c r="E189" s="13"/>
-      <c r="F189" s="13"/>
-      <c r="G189" s="13"/>
-      <c r="H189" s="13"/>
-      <c r="I189" s="13"/>
-      <c r="J189" s="13"/>
-      <c r="K189" s="13"/>
-      <c r="L189" s="13"/>
-      <c r="M189" s="13"/>
-      <c r="N189" s="13"/>
-      <c r="O189" s="13"/>
-      <c r="P189" s="13"/>
-      <c r="Q189" s="13"/>
-      <c r="R189" s="13"/>
       <c r="S189" s="6"/>
       <c r="T189" s="6"/>
     </row>
     <row r="190" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A190" s="5"/>
       <c r="B190" s="5"/>
-      <c r="C190" s="13"/>
-      <c r="D190" s="13"/>
-      <c r="E190" s="13"/>
-      <c r="F190" s="13"/>
-      <c r="G190" s="13"/>
-      <c r="H190" s="13"/>
-      <c r="I190" s="13"/>
-      <c r="J190" s="13"/>
-      <c r="K190" s="13"/>
-      <c r="L190" s="13"/>
-      <c r="M190" s="13"/>
-      <c r="N190" s="13"/>
-      <c r="O190" s="13"/>
-      <c r="P190" s="13"/>
-      <c r="Q190" s="13"/>
-      <c r="R190" s="13"/>
       <c r="S190" s="6"/>
       <c r="T190" s="6"/>
     </row>
@@ -8806,46 +6578,10 @@
     </row>
     <row r="192" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A192" s="5"/>
-      <c r="B192" s="13"/>
-      <c r="C192" s="13"/>
-      <c r="D192" s="13"/>
-      <c r="E192" s="13"/>
-      <c r="F192" s="13"/>
-      <c r="G192" s="13"/>
-      <c r="H192" s="13"/>
-      <c r="I192" s="13"/>
-      <c r="J192" s="13"/>
-      <c r="K192" s="13"/>
-      <c r="L192" s="13"/>
-      <c r="M192" s="13"/>
-      <c r="N192" s="13"/>
-      <c r="O192" s="13"/>
-      <c r="P192" s="13"/>
-      <c r="Q192" s="13"/>
-      <c r="R192" s="13"/>
-      <c r="S192" s="13"/>
       <c r="T192" s="6"/>
     </row>
     <row r="193" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A193" s="5"/>
-      <c r="B193" s="13"/>
-      <c r="C193" s="13"/>
-      <c r="D193" s="13"/>
-      <c r="E193" s="13"/>
-      <c r="F193" s="13"/>
-      <c r="G193" s="13"/>
-      <c r="H193" s="13"/>
-      <c r="I193" s="13"/>
-      <c r="J193" s="13"/>
-      <c r="K193" s="13"/>
-      <c r="L193" s="13"/>
-      <c r="M193" s="13"/>
-      <c r="N193" s="13"/>
-      <c r="O193" s="13"/>
-      <c r="P193" s="13"/>
-      <c r="Q193" s="13"/>
-      <c r="R193" s="13"/>
-      <c r="S193" s="13"/>
       <c r="T193" s="6"/>
     </row>
     <row r="194" spans="1:20" x14ac:dyDescent="0.25">
@@ -8875,660 +6611,180 @@
     <row r="195" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A195" s="5"/>
       <c r="B195" s="5"/>
-      <c r="C195" s="13"/>
-      <c r="D195" s="13"/>
-      <c r="E195" s="13"/>
-      <c r="F195" s="13"/>
-      <c r="G195" s="13"/>
-      <c r="H195" s="13"/>
-      <c r="I195" s="13"/>
-      <c r="J195" s="13"/>
-      <c r="K195" s="13"/>
-      <c r="L195" s="13"/>
-      <c r="M195" s="13"/>
-      <c r="N195" s="13"/>
-      <c r="O195" s="13"/>
-      <c r="P195" s="13"/>
-      <c r="Q195" s="13"/>
-      <c r="R195" s="13"/>
       <c r="S195" s="6"/>
       <c r="T195" s="6"/>
     </row>
     <row r="196" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A196" s="5"/>
       <c r="B196" s="5"/>
-      <c r="C196" s="13"/>
-      <c r="D196" s="13"/>
-      <c r="E196" s="13"/>
-      <c r="F196" s="13"/>
-      <c r="G196" s="13"/>
-      <c r="H196" s="13"/>
-      <c r="I196" s="13"/>
-      <c r="J196" s="13"/>
-      <c r="K196" s="13"/>
-      <c r="L196" s="13"/>
-      <c r="M196" s="13"/>
-      <c r="N196" s="13"/>
-      <c r="O196" s="13"/>
-      <c r="P196" s="13"/>
-      <c r="Q196" s="13"/>
-      <c r="R196" s="13"/>
       <c r="S196" s="6"/>
       <c r="T196" s="6"/>
     </row>
     <row r="197" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A197" s="5"/>
       <c r="B197" s="5"/>
-      <c r="C197" s="13"/>
-      <c r="D197" s="13"/>
-      <c r="E197" s="13"/>
-      <c r="F197" s="13"/>
-      <c r="G197" s="13"/>
-      <c r="H197" s="13"/>
-      <c r="I197" s="13"/>
-      <c r="J197" s="13"/>
-      <c r="K197" s="13"/>
-      <c r="L197" s="13"/>
-      <c r="M197" s="13"/>
-      <c r="N197" s="13"/>
-      <c r="O197" s="13"/>
-      <c r="P197" s="13"/>
-      <c r="Q197" s="13"/>
-      <c r="R197" s="13"/>
       <c r="S197" s="6"/>
       <c r="T197" s="6"/>
     </row>
     <row r="198" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A198" s="5"/>
       <c r="B198" s="5"/>
-      <c r="C198" s="13"/>
-      <c r="D198" s="13"/>
-      <c r="E198" s="13"/>
-      <c r="F198" s="13"/>
-      <c r="G198" s="13"/>
-      <c r="H198" s="13"/>
-      <c r="I198" s="13"/>
-      <c r="J198" s="13"/>
-      <c r="K198" s="13"/>
-      <c r="L198" s="13"/>
-      <c r="M198" s="13"/>
-      <c r="N198" s="13"/>
-      <c r="O198" s="13"/>
-      <c r="P198" s="13"/>
-      <c r="Q198" s="13"/>
-      <c r="R198" s="13"/>
       <c r="S198" s="6"/>
       <c r="T198" s="6"/>
     </row>
     <row r="199" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A199" s="5"/>
       <c r="B199" s="5"/>
-      <c r="C199" s="13"/>
-      <c r="D199" s="13"/>
-      <c r="E199" s="13"/>
-      <c r="F199" s="13"/>
-      <c r="G199" s="13"/>
-      <c r="H199" s="13"/>
-      <c r="I199" s="13"/>
-      <c r="J199" s="13"/>
-      <c r="K199" s="13"/>
-      <c r="L199" s="13"/>
-      <c r="M199" s="13"/>
-      <c r="N199" s="13"/>
-      <c r="O199" s="13"/>
-      <c r="P199" s="13"/>
-      <c r="Q199" s="13"/>
-      <c r="R199" s="13"/>
       <c r="S199" s="6"/>
       <c r="T199" s="6"/>
     </row>
     <row r="200" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A200" s="5"/>
       <c r="B200" s="5"/>
-      <c r="C200" s="13"/>
-      <c r="D200" s="13"/>
-      <c r="E200" s="13"/>
-      <c r="F200" s="13"/>
-      <c r="G200" s="13"/>
-      <c r="H200" s="13"/>
-      <c r="I200" s="13"/>
-      <c r="J200" s="13"/>
-      <c r="K200" s="13"/>
-      <c r="L200" s="13"/>
-      <c r="M200" s="13"/>
-      <c r="N200" s="13"/>
-      <c r="O200" s="13"/>
-      <c r="P200" s="13"/>
-      <c r="Q200" s="13"/>
-      <c r="R200" s="13"/>
       <c r="S200" s="6"/>
       <c r="T200" s="6"/>
     </row>
     <row r="201" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A201" s="5"/>
       <c r="B201" s="5"/>
-      <c r="C201" s="13"/>
-      <c r="D201" s="13"/>
-      <c r="E201" s="13"/>
-      <c r="F201" s="13"/>
-      <c r="G201" s="13"/>
-      <c r="H201" s="13"/>
-      <c r="I201" s="13"/>
-      <c r="J201" s="13"/>
-      <c r="K201" s="13"/>
-      <c r="L201" s="13"/>
-      <c r="M201" s="13"/>
-      <c r="N201" s="13"/>
-      <c r="O201" s="13"/>
-      <c r="P201" s="13"/>
-      <c r="Q201" s="13"/>
-      <c r="R201" s="13"/>
       <c r="S201" s="6"/>
       <c r="T201" s="6"/>
     </row>
     <row r="202" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A202" s="5"/>
       <c r="B202" s="5"/>
-      <c r="C202" s="13"/>
-      <c r="D202" s="13"/>
-      <c r="E202" s="13"/>
-      <c r="F202" s="13"/>
-      <c r="G202" s="13"/>
-      <c r="H202" s="13"/>
-      <c r="I202" s="13"/>
-      <c r="J202" s="13"/>
-      <c r="K202" s="13"/>
-      <c r="L202" s="13"/>
-      <c r="M202" s="13"/>
-      <c r="N202" s="13"/>
-      <c r="O202" s="13"/>
-      <c r="P202" s="13"/>
-      <c r="Q202" s="13"/>
-      <c r="R202" s="13"/>
       <c r="S202" s="6"/>
       <c r="T202" s="6"/>
     </row>
     <row r="203" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A203" s="5"/>
       <c r="B203" s="5"/>
-      <c r="C203" s="13"/>
-      <c r="D203" s="13"/>
-      <c r="E203" s="13"/>
-      <c r="F203" s="13"/>
-      <c r="G203" s="13"/>
-      <c r="H203" s="13"/>
-      <c r="I203" s="13"/>
-      <c r="J203" s="13"/>
-      <c r="K203" s="13"/>
-      <c r="L203" s="13"/>
-      <c r="M203" s="13"/>
-      <c r="N203" s="13"/>
-      <c r="O203" s="13"/>
-      <c r="P203" s="13"/>
-      <c r="Q203" s="13"/>
-      <c r="R203" s="13"/>
       <c r="S203" s="6"/>
       <c r="T203" s="6"/>
     </row>
     <row r="204" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A204" s="5"/>
       <c r="B204" s="5"/>
-      <c r="C204" s="13"/>
-      <c r="D204" s="13"/>
-      <c r="E204" s="13"/>
-      <c r="F204" s="13"/>
-      <c r="G204" s="13"/>
-      <c r="H204" s="13"/>
-      <c r="I204" s="13"/>
-      <c r="J204" s="13"/>
-      <c r="K204" s="13"/>
-      <c r="L204" s="13"/>
-      <c r="M204" s="13"/>
-      <c r="N204" s="13"/>
-      <c r="O204" s="13"/>
-      <c r="P204" s="13"/>
-      <c r="Q204" s="13"/>
-      <c r="R204" s="13"/>
       <c r="S204" s="6"/>
       <c r="T204" s="6"/>
     </row>
     <row r="205" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A205" s="5"/>
       <c r="B205" s="5"/>
-      <c r="C205" s="13"/>
-      <c r="D205" s="13"/>
-      <c r="E205" s="13"/>
-      <c r="F205" s="13"/>
-      <c r="G205" s="13"/>
-      <c r="H205" s="13"/>
-      <c r="I205" s="13"/>
-      <c r="J205" s="13"/>
-      <c r="K205" s="13"/>
-      <c r="L205" s="13"/>
-      <c r="M205" s="13"/>
-      <c r="N205" s="13"/>
-      <c r="O205" s="13"/>
-      <c r="P205" s="13"/>
-      <c r="Q205" s="13"/>
-      <c r="R205" s="13"/>
       <c r="S205" s="6"/>
       <c r="T205" s="6"/>
     </row>
     <row r="206" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A206" s="5"/>
       <c r="B206" s="5"/>
-      <c r="C206" s="13"/>
-      <c r="D206" s="13"/>
-      <c r="E206" s="13"/>
-      <c r="F206" s="13"/>
-      <c r="G206" s="13"/>
-      <c r="H206" s="13"/>
-      <c r="I206" s="13"/>
-      <c r="J206" s="13"/>
-      <c r="K206" s="13"/>
-      <c r="L206" s="13"/>
-      <c r="M206" s="13"/>
-      <c r="N206" s="13"/>
-      <c r="O206" s="13"/>
-      <c r="P206" s="13"/>
-      <c r="Q206" s="13"/>
-      <c r="R206" s="13"/>
       <c r="S206" s="6"/>
       <c r="T206" s="6"/>
     </row>
     <row r="207" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A207" s="5"/>
       <c r="B207" s="5"/>
-      <c r="C207" s="13"/>
-      <c r="D207" s="13"/>
-      <c r="E207" s="13"/>
-      <c r="F207" s="13"/>
-      <c r="G207" s="13"/>
-      <c r="H207" s="13"/>
-      <c r="I207" s="13"/>
-      <c r="J207" s="13"/>
-      <c r="K207" s="13"/>
-      <c r="L207" s="13"/>
-      <c r="M207" s="13"/>
-      <c r="N207" s="13"/>
-      <c r="O207" s="13"/>
-      <c r="P207" s="13"/>
-      <c r="Q207" s="13"/>
-      <c r="R207" s="13"/>
       <c r="S207" s="6"/>
       <c r="T207" s="6"/>
     </row>
     <row r="208" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A208" s="5"/>
       <c r="B208" s="5"/>
-      <c r="C208" s="13"/>
-      <c r="D208" s="13"/>
-      <c r="E208" s="13"/>
-      <c r="F208" s="13"/>
-      <c r="G208" s="13"/>
-      <c r="H208" s="13"/>
-      <c r="I208" s="13"/>
-      <c r="J208" s="13"/>
-      <c r="K208" s="13"/>
-      <c r="L208" s="13"/>
-      <c r="M208" s="13"/>
-      <c r="N208" s="13"/>
-      <c r="O208" s="13"/>
-      <c r="P208" s="13"/>
-      <c r="Q208" s="13"/>
-      <c r="R208" s="13"/>
       <c r="S208" s="6"/>
       <c r="T208" s="6"/>
     </row>
     <row r="209" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A209" s="5"/>
       <c r="B209" s="5"/>
-      <c r="C209" s="13"/>
-      <c r="D209" s="13"/>
-      <c r="E209" s="13"/>
-      <c r="F209" s="13"/>
-      <c r="G209" s="13"/>
-      <c r="H209" s="13"/>
-      <c r="I209" s="13"/>
-      <c r="J209" s="13"/>
-      <c r="K209" s="13"/>
-      <c r="L209" s="13"/>
-      <c r="M209" s="13"/>
-      <c r="N209" s="13"/>
-      <c r="O209" s="13"/>
-      <c r="P209" s="13"/>
-      <c r="Q209" s="13"/>
-      <c r="R209" s="13"/>
       <c r="S209" s="6"/>
       <c r="T209" s="6"/>
     </row>
     <row r="210" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A210" s="5"/>
       <c r="B210" s="5"/>
-      <c r="C210" s="13"/>
-      <c r="D210" s="13"/>
-      <c r="E210" s="13"/>
-      <c r="F210" s="13"/>
-      <c r="G210" s="13"/>
-      <c r="H210" s="13"/>
-      <c r="I210" s="13"/>
-      <c r="J210" s="13"/>
-      <c r="K210" s="13"/>
-      <c r="L210" s="13"/>
-      <c r="M210" s="13"/>
-      <c r="N210" s="13"/>
-      <c r="O210" s="13"/>
-      <c r="P210" s="13"/>
-      <c r="Q210" s="13"/>
-      <c r="R210" s="13"/>
       <c r="S210" s="6"/>
       <c r="T210" s="6"/>
     </row>
     <row r="211" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A211" s="5"/>
       <c r="B211" s="5"/>
-      <c r="C211" s="13"/>
-      <c r="D211" s="13"/>
-      <c r="E211" s="13"/>
-      <c r="F211" s="13"/>
-      <c r="G211" s="13"/>
-      <c r="H211" s="13"/>
-      <c r="I211" s="13"/>
-      <c r="J211" s="13"/>
-      <c r="K211" s="13"/>
-      <c r="L211" s="13"/>
-      <c r="M211" s="13"/>
-      <c r="N211" s="13"/>
-      <c r="O211" s="13"/>
-      <c r="P211" s="13"/>
-      <c r="Q211" s="13"/>
-      <c r="R211" s="13"/>
       <c r="S211" s="6"/>
       <c r="T211" s="6"/>
     </row>
     <row r="212" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A212" s="5"/>
       <c r="B212" s="5"/>
-      <c r="C212" s="13"/>
-      <c r="D212" s="13"/>
-      <c r="E212" s="13"/>
-      <c r="F212" s="13"/>
-      <c r="G212" s="13"/>
-      <c r="H212" s="13"/>
-      <c r="I212" s="13"/>
-      <c r="J212" s="13"/>
-      <c r="K212" s="13"/>
-      <c r="L212" s="13"/>
-      <c r="M212" s="13"/>
-      <c r="N212" s="13"/>
-      <c r="O212" s="13"/>
-      <c r="P212" s="13"/>
-      <c r="Q212" s="13"/>
-      <c r="R212" s="13"/>
       <c r="S212" s="6"/>
       <c r="T212" s="6"/>
     </row>
     <row r="213" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A213" s="5"/>
       <c r="B213" s="5"/>
-      <c r="C213" s="13"/>
-      <c r="D213" s="13"/>
-      <c r="E213" s="13"/>
-      <c r="F213" s="13"/>
-      <c r="G213" s="13"/>
-      <c r="H213" s="13"/>
-      <c r="I213" s="13"/>
-      <c r="J213" s="13"/>
-      <c r="K213" s="13"/>
-      <c r="L213" s="13"/>
-      <c r="M213" s="13"/>
-      <c r="N213" s="13"/>
-      <c r="O213" s="13"/>
-      <c r="P213" s="13"/>
-      <c r="Q213" s="13"/>
-      <c r="R213" s="13"/>
       <c r="S213" s="6"/>
       <c r="T213" s="6"/>
     </row>
     <row r="214" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A214" s="5"/>
       <c r="B214" s="5"/>
-      <c r="C214" s="13"/>
-      <c r="D214" s="13"/>
-      <c r="E214" s="13"/>
-      <c r="F214" s="13"/>
-      <c r="G214" s="13"/>
-      <c r="H214" s="13"/>
-      <c r="I214" s="13"/>
-      <c r="J214" s="13"/>
-      <c r="K214" s="13"/>
-      <c r="L214" s="13"/>
-      <c r="M214" s="13"/>
-      <c r="N214" s="13"/>
-      <c r="O214" s="13"/>
-      <c r="P214" s="13"/>
-      <c r="Q214" s="13"/>
-      <c r="R214" s="13"/>
       <c r="S214" s="6"/>
       <c r="T214" s="6"/>
     </row>
     <row r="215" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A215" s="5"/>
       <c r="B215" s="5"/>
-      <c r="C215" s="13"/>
-      <c r="D215" s="13"/>
-      <c r="E215" s="13"/>
-      <c r="F215" s="13"/>
-      <c r="G215" s="13"/>
-      <c r="H215" s="13"/>
-      <c r="I215" s="13"/>
-      <c r="J215" s="13"/>
-      <c r="K215" s="13"/>
-      <c r="L215" s="13"/>
-      <c r="M215" s="13"/>
-      <c r="N215" s="13"/>
-      <c r="O215" s="13"/>
-      <c r="P215" s="13"/>
-      <c r="Q215" s="13"/>
-      <c r="R215" s="13"/>
       <c r="S215" s="6"/>
       <c r="T215" s="6"/>
     </row>
     <row r="216" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A216" s="5"/>
       <c r="B216" s="5"/>
-      <c r="C216" s="13"/>
-      <c r="D216" s="13"/>
-      <c r="E216" s="13"/>
-      <c r="F216" s="13"/>
-      <c r="G216" s="13"/>
-      <c r="H216" s="13"/>
-      <c r="I216" s="13"/>
-      <c r="J216" s="13"/>
-      <c r="K216" s="13"/>
-      <c r="L216" s="13"/>
-      <c r="M216" s="13"/>
-      <c r="N216" s="13"/>
-      <c r="O216" s="13"/>
-      <c r="P216" s="13"/>
-      <c r="Q216" s="13"/>
-      <c r="R216" s="13"/>
       <c r="S216" s="6"/>
       <c r="T216" s="6"/>
     </row>
     <row r="217" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A217" s="5"/>
       <c r="B217" s="5"/>
-      <c r="C217" s="13"/>
-      <c r="D217" s="13"/>
-      <c r="E217" s="13"/>
-      <c r="F217" s="13"/>
-      <c r="G217" s="13"/>
-      <c r="H217" s="13"/>
-      <c r="I217" s="13"/>
-      <c r="J217" s="13"/>
-      <c r="K217" s="13"/>
-      <c r="L217" s="13"/>
-      <c r="M217" s="13"/>
-      <c r="N217" s="13"/>
-      <c r="O217" s="13"/>
-      <c r="P217" s="13"/>
-      <c r="Q217" s="13"/>
-      <c r="R217" s="13"/>
       <c r="S217" s="6"/>
       <c r="T217" s="6"/>
     </row>
     <row r="218" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A218" s="5"/>
       <c r="B218" s="5"/>
-      <c r="C218" s="13"/>
-      <c r="D218" s="13"/>
-      <c r="E218" s="13"/>
-      <c r="F218" s="13"/>
-      <c r="G218" s="13"/>
-      <c r="H218" s="13"/>
-      <c r="I218" s="13"/>
-      <c r="J218" s="13"/>
-      <c r="K218" s="13"/>
-      <c r="L218" s="13"/>
-      <c r="M218" s="13"/>
-      <c r="N218" s="13"/>
-      <c r="O218" s="13"/>
-      <c r="P218" s="13"/>
-      <c r="Q218" s="13"/>
-      <c r="R218" s="13"/>
       <c r="S218" s="6"/>
       <c r="T218" s="6"/>
     </row>
     <row r="219" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A219" s="5"/>
       <c r="B219" s="5"/>
-      <c r="C219" s="13"/>
-      <c r="D219" s="13"/>
-      <c r="E219" s="13"/>
-      <c r="F219" s="13"/>
-      <c r="G219" s="13"/>
-      <c r="H219" s="13"/>
-      <c r="I219" s="13"/>
-      <c r="J219" s="13"/>
-      <c r="K219" s="13"/>
-      <c r="L219" s="13"/>
-      <c r="M219" s="13"/>
-      <c r="N219" s="13"/>
-      <c r="O219" s="13"/>
-      <c r="P219" s="13"/>
-      <c r="Q219" s="13"/>
-      <c r="R219" s="13"/>
       <c r="S219" s="6"/>
       <c r="T219" s="6"/>
     </row>
     <row r="220" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A220" s="5"/>
       <c r="B220" s="5"/>
-      <c r="C220" s="13"/>
-      <c r="D220" s="13"/>
-      <c r="E220" s="13"/>
-      <c r="F220" s="13"/>
-      <c r="G220" s="13"/>
-      <c r="H220" s="13"/>
-      <c r="I220" s="13"/>
-      <c r="J220" s="13"/>
-      <c r="K220" s="13"/>
-      <c r="L220" s="13"/>
-      <c r="M220" s="13"/>
-      <c r="N220" s="13"/>
-      <c r="O220" s="13"/>
-      <c r="P220" s="13"/>
-      <c r="Q220" s="13"/>
-      <c r="R220" s="13"/>
       <c r="S220" s="6"/>
       <c r="T220" s="6"/>
     </row>
     <row r="221" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A221" s="5"/>
       <c r="B221" s="5"/>
-      <c r="C221" s="13"/>
-      <c r="D221" s="13"/>
-      <c r="E221" s="13"/>
-      <c r="F221" s="13"/>
-      <c r="G221" s="13"/>
-      <c r="H221" s="13"/>
-      <c r="I221" s="13"/>
-      <c r="J221" s="13"/>
-      <c r="K221" s="13"/>
-      <c r="L221" s="13"/>
-      <c r="M221" s="13"/>
-      <c r="N221" s="13"/>
-      <c r="O221" s="13"/>
-      <c r="P221" s="13"/>
-      <c r="Q221" s="13"/>
-      <c r="R221" s="13"/>
       <c r="S221" s="6"/>
       <c r="T221" s="6"/>
     </row>
     <row r="222" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A222" s="5"/>
       <c r="B222" s="5"/>
-      <c r="C222" s="13"/>
-      <c r="D222" s="13"/>
-      <c r="E222" s="13"/>
-      <c r="F222" s="13"/>
-      <c r="G222" s="13"/>
-      <c r="H222" s="13"/>
-      <c r="I222" s="13"/>
-      <c r="J222" s="13"/>
-      <c r="K222" s="13"/>
-      <c r="L222" s="13"/>
-      <c r="M222" s="13"/>
-      <c r="N222" s="13"/>
-      <c r="O222" s="13"/>
-      <c r="P222" s="13"/>
-      <c r="Q222" s="13"/>
-      <c r="R222" s="13"/>
       <c r="S222" s="6"/>
       <c r="T222" s="6"/>
     </row>
     <row r="223" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A223" s="5"/>
       <c r="B223" s="5"/>
-      <c r="C223" s="13"/>
-      <c r="D223" s="13"/>
-      <c r="E223" s="13"/>
-      <c r="F223" s="13"/>
-      <c r="G223" s="13"/>
-      <c r="H223" s="13"/>
-      <c r="I223" s="13"/>
-      <c r="J223" s="13"/>
-      <c r="K223" s="13"/>
-      <c r="L223" s="13"/>
-      <c r="M223" s="13"/>
-      <c r="N223" s="13"/>
-      <c r="O223" s="13"/>
-      <c r="P223" s="13"/>
-      <c r="Q223" s="13"/>
-      <c r="R223" s="13"/>
       <c r="S223" s="6"/>
       <c r="T223" s="6"/>
     </row>
     <row r="224" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A224" s="5"/>
       <c r="B224" s="5"/>
-      <c r="C224" s="13"/>
-      <c r="D224" s="13"/>
-      <c r="E224" s="13"/>
-      <c r="F224" s="13"/>
-      <c r="G224" s="13"/>
-      <c r="H224" s="13"/>
-      <c r="I224" s="13"/>
-      <c r="J224" s="13"/>
-      <c r="K224" s="13"/>
-      <c r="L224" s="13"/>
-      <c r="M224" s="13"/>
-      <c r="N224" s="13"/>
-      <c r="O224" s="13"/>
-      <c r="P224" s="13"/>
-      <c r="Q224" s="13"/>
-      <c r="R224" s="13"/>
       <c r="S224" s="6"/>
       <c r="T224" s="6"/>
     </row>
@@ -9537,638 +6793,174 @@
       <c r="B225" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C225" s="13"/>
-      <c r="D225" s="13"/>
-      <c r="E225" s="13"/>
-      <c r="F225" s="13"/>
-      <c r="G225" s="13"/>
-      <c r="H225" s="13"/>
-      <c r="I225" s="13"/>
-      <c r="J225" s="13"/>
-      <c r="K225" s="13"/>
-      <c r="L225" s="13"/>
-      <c r="M225" s="13"/>
-      <c r="N225" s="13"/>
-      <c r="O225" s="13"/>
-      <c r="P225" s="13"/>
-      <c r="Q225" s="13"/>
-      <c r="R225" s="13"/>
       <c r="S225" s="6"/>
       <c r="T225" s="6"/>
     </row>
     <row r="226" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A226" s="5"/>
       <c r="B226" s="5"/>
-      <c r="C226" s="13"/>
-      <c r="D226" s="13"/>
-      <c r="E226" s="13"/>
-      <c r="F226" s="13"/>
-      <c r="G226" s="13"/>
-      <c r="H226" s="13"/>
-      <c r="I226" s="13"/>
-      <c r="J226" s="13"/>
-      <c r="K226" s="13"/>
-      <c r="L226" s="13"/>
-      <c r="M226" s="13"/>
-      <c r="N226" s="13"/>
-      <c r="O226" s="13"/>
-      <c r="P226" s="13"/>
-      <c r="Q226" s="13"/>
-      <c r="R226" s="13"/>
       <c r="S226" s="6"/>
       <c r="T226" s="6"/>
     </row>
     <row r="227" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A227" s="5"/>
       <c r="B227" s="5"/>
-      <c r="C227" s="13"/>
-      <c r="D227" s="13"/>
-      <c r="E227" s="13"/>
-      <c r="F227" s="13"/>
-      <c r="G227" s="13"/>
-      <c r="H227" s="13"/>
-      <c r="I227" s="13"/>
-      <c r="J227" s="13"/>
-      <c r="K227" s="13"/>
-      <c r="L227" s="13"/>
-      <c r="M227" s="13"/>
-      <c r="N227" s="13"/>
-      <c r="O227" s="13"/>
-      <c r="P227" s="13"/>
-      <c r="Q227" s="13"/>
-      <c r="R227" s="13"/>
       <c r="S227" s="6"/>
       <c r="T227" s="6"/>
     </row>
     <row r="228" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A228" s="5"/>
       <c r="B228" s="5"/>
-      <c r="C228" s="13"/>
-      <c r="D228" s="13"/>
-      <c r="E228" s="13"/>
-      <c r="F228" s="13"/>
-      <c r="G228" s="13"/>
-      <c r="H228" s="13"/>
-      <c r="I228" s="13"/>
-      <c r="J228" s="13"/>
-      <c r="K228" s="13"/>
-      <c r="L228" s="13"/>
-      <c r="M228" s="13"/>
-      <c r="N228" s="13"/>
-      <c r="O228" s="13"/>
-      <c r="P228" s="13"/>
-      <c r="Q228" s="13"/>
-      <c r="R228" s="13"/>
       <c r="S228" s="6"/>
       <c r="T228" s="6"/>
     </row>
     <row r="229" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A229" s="5"/>
       <c r="B229" s="5"/>
-      <c r="C229" s="13"/>
-      <c r="D229" s="13"/>
-      <c r="E229" s="13"/>
-      <c r="F229" s="13"/>
-      <c r="G229" s="13"/>
-      <c r="H229" s="13"/>
-      <c r="I229" s="13"/>
-      <c r="J229" s="13"/>
-      <c r="K229" s="13"/>
-      <c r="L229" s="13"/>
-      <c r="M229" s="13"/>
-      <c r="N229" s="13"/>
-      <c r="O229" s="13"/>
-      <c r="P229" s="13"/>
-      <c r="Q229" s="13"/>
-      <c r="R229" s="13"/>
       <c r="S229" s="6"/>
       <c r="T229" s="6"/>
     </row>
     <row r="230" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A230" s="5"/>
       <c r="B230" s="5"/>
-      <c r="C230" s="13"/>
-      <c r="D230" s="13"/>
-      <c r="E230" s="13"/>
-      <c r="F230" s="13"/>
-      <c r="G230" s="13"/>
-      <c r="H230" s="13"/>
-      <c r="I230" s="13"/>
-      <c r="J230" s="13"/>
-      <c r="K230" s="13"/>
-      <c r="L230" s="13"/>
-      <c r="M230" s="13"/>
-      <c r="N230" s="13"/>
-      <c r="O230" s="13"/>
-      <c r="P230" s="13"/>
-      <c r="Q230" s="13"/>
-      <c r="R230" s="13"/>
       <c r="S230" s="6"/>
       <c r="T230" s="6"/>
     </row>
     <row r="231" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A231" s="5"/>
       <c r="B231" s="5"/>
-      <c r="C231" s="13"/>
-      <c r="D231" s="13"/>
-      <c r="E231" s="13"/>
-      <c r="F231" s="13"/>
-      <c r="G231" s="13"/>
-      <c r="H231" s="13"/>
-      <c r="I231" s="13"/>
-      <c r="J231" s="13"/>
-      <c r="K231" s="13"/>
-      <c r="L231" s="13"/>
-      <c r="M231" s="13"/>
-      <c r="N231" s="13"/>
-      <c r="O231" s="13"/>
-      <c r="P231" s="13"/>
-      <c r="Q231" s="13"/>
-      <c r="R231" s="13"/>
       <c r="S231" s="6"/>
       <c r="T231" s="6"/>
     </row>
     <row r="232" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A232" s="5"/>
       <c r="B232" s="5"/>
-      <c r="C232" s="13"/>
-      <c r="D232" s="13"/>
-      <c r="E232" s="13"/>
-      <c r="F232" s="13"/>
-      <c r="G232" s="13"/>
-      <c r="H232" s="13"/>
-      <c r="I232" s="13"/>
-      <c r="J232" s="13"/>
-      <c r="K232" s="13"/>
-      <c r="L232" s="13"/>
-      <c r="M232" s="13"/>
-      <c r="N232" s="13"/>
-      <c r="O232" s="13"/>
-      <c r="P232" s="13"/>
-      <c r="Q232" s="13"/>
-      <c r="R232" s="13"/>
       <c r="S232" s="6"/>
       <c r="T232" s="6"/>
     </row>
     <row r="233" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A233" s="5"/>
       <c r="B233" s="5"/>
-      <c r="C233" s="13"/>
-      <c r="D233" s="13"/>
-      <c r="E233" s="13"/>
-      <c r="F233" s="13"/>
-      <c r="G233" s="13"/>
-      <c r="H233" s="13"/>
-      <c r="I233" s="13"/>
-      <c r="J233" s="13"/>
-      <c r="K233" s="13"/>
-      <c r="L233" s="13"/>
-      <c r="M233" s="13"/>
-      <c r="N233" s="13"/>
-      <c r="O233" s="13"/>
-      <c r="P233" s="13"/>
-      <c r="Q233" s="13"/>
-      <c r="R233" s="13"/>
       <c r="S233" s="6"/>
       <c r="T233" s="6"/>
     </row>
     <row r="234" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A234" s="5"/>
       <c r="B234" s="5"/>
-      <c r="C234" s="13"/>
-      <c r="D234" s="13"/>
-      <c r="E234" s="13"/>
-      <c r="F234" s="13"/>
-      <c r="G234" s="13"/>
-      <c r="H234" s="13"/>
-      <c r="I234" s="13"/>
-      <c r="J234" s="13"/>
-      <c r="K234" s="13"/>
-      <c r="L234" s="13"/>
-      <c r="M234" s="13"/>
-      <c r="N234" s="13"/>
-      <c r="O234" s="13"/>
-      <c r="P234" s="13"/>
-      <c r="Q234" s="13"/>
-      <c r="R234" s="13"/>
       <c r="S234" s="6"/>
       <c r="T234" s="6"/>
     </row>
     <row r="235" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A235" s="5"/>
       <c r="B235" s="5"/>
-      <c r="C235" s="13"/>
-      <c r="D235" s="13"/>
-      <c r="E235" s="13"/>
-      <c r="F235" s="13"/>
-      <c r="G235" s="13"/>
-      <c r="H235" s="13"/>
-      <c r="I235" s="13"/>
-      <c r="J235" s="13"/>
-      <c r="K235" s="13"/>
-      <c r="L235" s="13"/>
-      <c r="M235" s="13"/>
-      <c r="N235" s="13"/>
-      <c r="O235" s="13"/>
-      <c r="P235" s="13"/>
-      <c r="Q235" s="13"/>
-      <c r="R235" s="13"/>
       <c r="S235" s="6"/>
       <c r="T235" s="6"/>
     </row>
     <row r="236" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A236" s="5"/>
       <c r="B236" s="5"/>
-      <c r="C236" s="13"/>
-      <c r="D236" s="13"/>
-      <c r="E236" s="13"/>
-      <c r="F236" s="13"/>
-      <c r="G236" s="13"/>
-      <c r="H236" s="13"/>
-      <c r="I236" s="13"/>
-      <c r="J236" s="13"/>
-      <c r="K236" s="13"/>
-      <c r="L236" s="13"/>
-      <c r="M236" s="13"/>
-      <c r="N236" s="13"/>
-      <c r="O236" s="13"/>
-      <c r="P236" s="13"/>
-      <c r="Q236" s="13"/>
-      <c r="R236" s="13"/>
       <c r="S236" s="6"/>
       <c r="T236" s="6"/>
     </row>
     <row r="237" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A237" s="5"/>
       <c r="B237" s="5"/>
-      <c r="C237" s="13"/>
-      <c r="D237" s="13"/>
-      <c r="E237" s="13"/>
-      <c r="F237" s="13"/>
-      <c r="G237" s="13"/>
-      <c r="H237" s="13"/>
-      <c r="I237" s="13"/>
-      <c r="J237" s="13"/>
-      <c r="K237" s="13"/>
-      <c r="L237" s="13"/>
-      <c r="M237" s="13"/>
-      <c r="N237" s="13"/>
-      <c r="O237" s="13"/>
-      <c r="P237" s="13"/>
-      <c r="Q237" s="13"/>
-      <c r="R237" s="13"/>
       <c r="S237" s="6"/>
       <c r="T237" s="6"/>
     </row>
     <row r="238" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A238" s="5"/>
       <c r="B238" s="5"/>
-      <c r="C238" s="13"/>
-      <c r="D238" s="13"/>
-      <c r="E238" s="13"/>
-      <c r="F238" s="13"/>
-      <c r="G238" s="13"/>
-      <c r="H238" s="13"/>
-      <c r="I238" s="13"/>
-      <c r="J238" s="13"/>
-      <c r="K238" s="13"/>
-      <c r="L238" s="13"/>
-      <c r="M238" s="13"/>
-      <c r="N238" s="13"/>
-      <c r="O238" s="13"/>
-      <c r="P238" s="13"/>
-      <c r="Q238" s="13"/>
-      <c r="R238" s="13"/>
       <c r="S238" s="6"/>
       <c r="T238" s="6"/>
     </row>
     <row r="239" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A239" s="5"/>
       <c r="B239" s="5"/>
-      <c r="C239" s="13"/>
-      <c r="D239" s="13"/>
-      <c r="E239" s="13"/>
-      <c r="F239" s="13"/>
-      <c r="G239" s="13"/>
-      <c r="H239" s="13"/>
-      <c r="I239" s="13"/>
-      <c r="J239" s="13"/>
-      <c r="K239" s="13"/>
-      <c r="L239" s="13"/>
-      <c r="M239" s="13"/>
-      <c r="N239" s="13"/>
-      <c r="O239" s="13"/>
-      <c r="P239" s="13"/>
-      <c r="Q239" s="13"/>
-      <c r="R239" s="13"/>
       <c r="S239" s="6"/>
       <c r="T239" s="6"/>
     </row>
     <row r="240" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A240" s="5"/>
       <c r="B240" s="5"/>
-      <c r="C240" s="13"/>
-      <c r="D240" s="13"/>
-      <c r="E240" s="13"/>
-      <c r="F240" s="13"/>
-      <c r="G240" s="13"/>
-      <c r="H240" s="13"/>
-      <c r="I240" s="13"/>
-      <c r="J240" s="13"/>
-      <c r="K240" s="13"/>
-      <c r="L240" s="13"/>
-      <c r="M240" s="13"/>
-      <c r="N240" s="13"/>
-      <c r="O240" s="13"/>
-      <c r="P240" s="13"/>
-      <c r="Q240" s="13"/>
-      <c r="R240" s="13"/>
       <c r="S240" s="6"/>
       <c r="T240" s="6"/>
     </row>
     <row r="241" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A241" s="5"/>
       <c r="B241" s="5"/>
-      <c r="C241" s="13"/>
-      <c r="D241" s="13"/>
-      <c r="E241" s="13"/>
-      <c r="F241" s="13"/>
-      <c r="G241" s="13"/>
-      <c r="H241" s="13"/>
-      <c r="I241" s="13"/>
-      <c r="J241" s="13"/>
-      <c r="K241" s="13"/>
-      <c r="L241" s="13"/>
-      <c r="M241" s="13"/>
-      <c r="N241" s="13"/>
-      <c r="O241" s="13"/>
-      <c r="P241" s="13"/>
-      <c r="Q241" s="13"/>
-      <c r="R241" s="13"/>
       <c r="S241" s="6"/>
       <c r="T241" s="6"/>
     </row>
     <row r="242" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A242" s="5"/>
       <c r="B242" s="5"/>
-      <c r="C242" s="13"/>
-      <c r="D242" s="13"/>
-      <c r="E242" s="13"/>
-      <c r="F242" s="13"/>
-      <c r="G242" s="13"/>
-      <c r="H242" s="13"/>
-      <c r="I242" s="13"/>
-      <c r="J242" s="13"/>
-      <c r="K242" s="13"/>
-      <c r="L242" s="13"/>
-      <c r="M242" s="13"/>
-      <c r="N242" s="13"/>
-      <c r="O242" s="13"/>
-      <c r="P242" s="13"/>
-      <c r="Q242" s="13"/>
-      <c r="R242" s="13"/>
       <c r="S242" s="6"/>
       <c r="T242" s="6"/>
     </row>
     <row r="243" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A243" s="5"/>
       <c r="B243" s="5"/>
-      <c r="C243" s="13"/>
-      <c r="D243" s="13"/>
-      <c r="E243" s="13"/>
-      <c r="F243" s="13"/>
-      <c r="G243" s="13"/>
-      <c r="H243" s="13"/>
-      <c r="I243" s="13"/>
-      <c r="J243" s="13"/>
-      <c r="K243" s="13"/>
-      <c r="L243" s="13"/>
-      <c r="M243" s="13"/>
-      <c r="N243" s="13"/>
-      <c r="O243" s="13"/>
-      <c r="P243" s="13"/>
-      <c r="Q243" s="13"/>
-      <c r="R243" s="13"/>
       <c r="S243" s="6"/>
       <c r="T243" s="6"/>
     </row>
     <row r="244" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A244" s="5"/>
       <c r="B244" s="5"/>
-      <c r="C244" s="13"/>
-      <c r="D244" s="13"/>
-      <c r="E244" s="13"/>
-      <c r="F244" s="13"/>
-      <c r="G244" s="13"/>
-      <c r="H244" s="13"/>
-      <c r="I244" s="13"/>
-      <c r="J244" s="13"/>
-      <c r="K244" s="13"/>
-      <c r="L244" s="13"/>
-      <c r="M244" s="13"/>
-      <c r="N244" s="13"/>
-      <c r="O244" s="13"/>
-      <c r="P244" s="13"/>
-      <c r="Q244" s="13"/>
-      <c r="R244" s="13"/>
       <c r="S244" s="6"/>
       <c r="T244" s="6"/>
     </row>
     <row r="245" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A245" s="5"/>
       <c r="B245" s="5"/>
-      <c r="C245" s="13"/>
-      <c r="D245" s="13"/>
-      <c r="E245" s="13"/>
-      <c r="F245" s="13"/>
-      <c r="G245" s="13"/>
-      <c r="H245" s="13"/>
-      <c r="I245" s="13"/>
-      <c r="J245" s="13"/>
-      <c r="K245" s="13"/>
-      <c r="L245" s="13"/>
-      <c r="M245" s="13"/>
-      <c r="N245" s="13"/>
-      <c r="O245" s="13"/>
-      <c r="P245" s="13"/>
-      <c r="Q245" s="13"/>
-      <c r="R245" s="13"/>
       <c r="S245" s="6"/>
       <c r="T245" s="6"/>
     </row>
     <row r="246" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A246" s="5"/>
       <c r="B246" s="5"/>
-      <c r="C246" s="13"/>
-      <c r="D246" s="13"/>
-      <c r="E246" s="13"/>
-      <c r="F246" s="13"/>
-      <c r="G246" s="13"/>
-      <c r="H246" s="13"/>
-      <c r="I246" s="13"/>
-      <c r="J246" s="13"/>
-      <c r="K246" s="13"/>
-      <c r="L246" s="13"/>
-      <c r="M246" s="13"/>
-      <c r="N246" s="13"/>
-      <c r="O246" s="13"/>
-      <c r="P246" s="13"/>
-      <c r="Q246" s="13"/>
-      <c r="R246" s="13"/>
       <c r="S246" s="6"/>
       <c r="T246" s="6"/>
     </row>
     <row r="247" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A247" s="5"/>
       <c r="B247" s="5"/>
-      <c r="C247" s="13"/>
-      <c r="D247" s="13"/>
-      <c r="E247" s="13"/>
-      <c r="F247" s="13"/>
-      <c r="G247" s="13"/>
-      <c r="H247" s="13"/>
-      <c r="I247" s="13"/>
-      <c r="J247" s="13"/>
-      <c r="K247" s="13"/>
-      <c r="L247" s="13"/>
-      <c r="M247" s="13"/>
-      <c r="N247" s="13"/>
-      <c r="O247" s="13"/>
-      <c r="P247" s="13"/>
-      <c r="Q247" s="13"/>
-      <c r="R247" s="13"/>
       <c r="S247" s="6"/>
       <c r="T247" s="6"/>
     </row>
     <row r="248" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A248" s="5"/>
       <c r="B248" s="5"/>
-      <c r="C248" s="13"/>
-      <c r="D248" s="13"/>
-      <c r="E248" s="13"/>
-      <c r="F248" s="13"/>
-      <c r="G248" s="13"/>
-      <c r="H248" s="13"/>
-      <c r="I248" s="13"/>
-      <c r="J248" s="13"/>
-      <c r="K248" s="13"/>
-      <c r="L248" s="13"/>
-      <c r="M248" s="13"/>
-      <c r="N248" s="13"/>
-      <c r="O248" s="13"/>
-      <c r="P248" s="13"/>
-      <c r="Q248" s="13"/>
-      <c r="R248" s="13"/>
       <c r="S248" s="6"/>
       <c r="T248" s="6"/>
     </row>
     <row r="249" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A249" s="5"/>
       <c r="B249" s="5"/>
-      <c r="C249" s="13"/>
-      <c r="D249" s="13"/>
-      <c r="E249" s="13"/>
-      <c r="F249" s="13"/>
-      <c r="G249" s="13"/>
-      <c r="H249" s="13"/>
-      <c r="I249" s="13"/>
-      <c r="J249" s="13"/>
-      <c r="K249" s="13"/>
-      <c r="L249" s="13"/>
-      <c r="M249" s="13"/>
-      <c r="N249" s="13"/>
-      <c r="O249" s="13"/>
-      <c r="P249" s="13"/>
-      <c r="Q249" s="13"/>
-      <c r="R249" s="13"/>
       <c r="S249" s="6"/>
       <c r="T249" s="6"/>
     </row>
     <row r="250" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A250" s="5"/>
       <c r="B250" s="5"/>
-      <c r="C250" s="13"/>
-      <c r="D250" s="13"/>
-      <c r="E250" s="13"/>
-      <c r="F250" s="13"/>
-      <c r="G250" s="13"/>
-      <c r="H250" s="13"/>
-      <c r="I250" s="13"/>
-      <c r="J250" s="13"/>
-      <c r="K250" s="13"/>
-      <c r="L250" s="13"/>
-      <c r="M250" s="13"/>
-      <c r="N250" s="13"/>
-      <c r="O250" s="13"/>
-      <c r="P250" s="13"/>
-      <c r="Q250" s="13"/>
-      <c r="R250" s="13"/>
       <c r="S250" s="6"/>
       <c r="T250" s="6"/>
     </row>
     <row r="251" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A251" s="5"/>
       <c r="B251" s="5"/>
-      <c r="C251" s="13"/>
-      <c r="D251" s="13"/>
-      <c r="E251" s="13"/>
-      <c r="F251" s="13"/>
-      <c r="G251" s="13"/>
-      <c r="H251" s="13"/>
-      <c r="I251" s="13"/>
-      <c r="J251" s="13"/>
-      <c r="K251" s="13"/>
-      <c r="L251" s="13"/>
-      <c r="M251" s="13"/>
-      <c r="N251" s="13"/>
-      <c r="O251" s="13"/>
-      <c r="P251" s="13"/>
-      <c r="Q251" s="13"/>
-      <c r="R251" s="13"/>
       <c r="S251" s="6"/>
       <c r="T251" s="6"/>
     </row>
     <row r="252" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A252" s="5"/>
       <c r="B252" s="5"/>
-      <c r="C252" s="13"/>
-      <c r="D252" s="13"/>
-      <c r="E252" s="13"/>
-      <c r="F252" s="13"/>
-      <c r="G252" s="13"/>
-      <c r="H252" s="13"/>
-      <c r="I252" s="13"/>
-      <c r="J252" s="13"/>
-      <c r="K252" s="13"/>
-      <c r="L252" s="13"/>
-      <c r="M252" s="13"/>
-      <c r="N252" s="13"/>
-      <c r="O252" s="13"/>
-      <c r="P252" s="13"/>
-      <c r="Q252" s="13"/>
-      <c r="R252" s="13"/>
       <c r="S252" s="6"/>
       <c r="T252" s="6"/>
     </row>
     <row r="253" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A253" s="5"/>
       <c r="B253" s="5"/>
-      <c r="C253" s="13"/>
-      <c r="D253" s="13"/>
-      <c r="E253" s="13"/>
-      <c r="F253" s="13"/>
-      <c r="G253" s="13"/>
-      <c r="H253" s="13"/>
-      <c r="I253" s="13"/>
-      <c r="J253" s="13"/>
-      <c r="K253" s="13"/>
-      <c r="L253" s="13"/>
-      <c r="M253" s="13"/>
-      <c r="N253" s="13"/>
-      <c r="O253" s="13"/>
-      <c r="P253" s="13"/>
-      <c r="Q253" s="13"/>
-      <c r="R253" s="13"/>
       <c r="S253" s="6"/>
       <c r="T253" s="6"/>
     </row>
@@ -10220,4 +7012,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105EBE37-F87C-407C-8CAD-25708265A35D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>